<commit_message>
Versión completa para entrega regional anual 2023
</commit_message>
<xml_diff>
--- a/SectoresRegionesAños.xlsx
+++ b/SectoresRegionesAños.xlsx
@@ -519,7 +519,7 @@
         <v>2596249028.367953</v>
       </c>
       <c r="F3" t="n">
-        <v>71815.57304762008</v>
+        <v>71815.57304762011</v>
       </c>
       <c r="G3" t="n">
         <v>535</v>
@@ -543,13 +543,13 @@
         </is>
       </c>
       <c r="D4" t="n">
-        <v>8016889.635061068</v>
+        <v>8016889.635061076</v>
       </c>
       <c r="E4" t="n">
-        <v>6689476865.087152</v>
+        <v>6689476865.087154</v>
       </c>
       <c r="F4" t="n">
-        <v>186206.8428017451</v>
+        <v>186206.842801745</v>
       </c>
       <c r="G4" t="n">
         <v>3414</v>
@@ -573,7 +573,7 @@
         </is>
       </c>
       <c r="D5" t="n">
-        <v>1257475.949354068</v>
+        <v>1257475.949354069</v>
       </c>
       <c r="E5" t="n">
         <v>1079525031.538227</v>
@@ -606,10 +606,10 @@
         <v>111743957.4764291</v>
       </c>
       <c r="E6" t="n">
-        <v>93605255144.22256</v>
+        <v>93605255144.22261</v>
       </c>
       <c r="F6" t="n">
-        <v>2606423.791336411</v>
+        <v>2606423.79133641</v>
       </c>
       <c r="G6" t="n">
         <v>9082</v>
@@ -633,7 +633,7 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>121944712.1061181</v>
+        <v>121944712.106118</v>
       </c>
       <c r="E7" t="n">
         <v>100748055672.2341</v>
@@ -663,10 +663,10 @@
         </is>
       </c>
       <c r="D8" t="n">
-        <v>80143501.4129349</v>
+        <v>80143501.41293502</v>
       </c>
       <c r="E8" t="n">
-        <v>67059518917.6581</v>
+        <v>67059518917.65807</v>
       </c>
       <c r="F8" t="n">
         <v>1865512.368336592</v>
@@ -696,10 +696,10 @@
         <v>107681028.4835678</v>
       </c>
       <c r="E9" t="n">
-        <v>91932227055.50014</v>
+        <v>91932227055.50015</v>
       </c>
       <c r="F9" t="n">
-        <v>2548738.879435055</v>
+        <v>2548738.879435054</v>
       </c>
       <c r="G9" t="n">
         <v>1942</v>
@@ -723,13 +723,13 @@
         </is>
       </c>
       <c r="D10" t="n">
-        <v>88401561.20560186</v>
+        <v>88401561.20560193</v>
       </c>
       <c r="E10" t="n">
-        <v>73830546895.55612</v>
+        <v>73830546895.55615</v>
       </c>
       <c r="F10" t="n">
-        <v>2055460.477919978</v>
+        <v>2055460.477919979</v>
       </c>
       <c r="G10" t="n">
         <v>17900</v>
@@ -753,13 +753,13 @@
         </is>
       </c>
       <c r="D11" t="n">
-        <v>539455.6714671609</v>
+        <v>539455.6714671608</v>
       </c>
       <c r="E11" t="n">
         <v>462712567.8444978</v>
       </c>
       <c r="F11" t="n">
-        <v>12796.48880601585</v>
+        <v>12796.48880601586</v>
       </c>
       <c r="G11" t="n">
         <v>633</v>
@@ -783,13 +783,13 @@
         </is>
       </c>
       <c r="D12" t="n">
-        <v>21304323.0854132</v>
+        <v>21304323.08541318</v>
       </c>
       <c r="E12" t="n">
         <v>17777364277.21906</v>
       </c>
       <c r="F12" t="n">
-        <v>494706.9305871958</v>
+        <v>494706.9305871961</v>
       </c>
       <c r="G12" t="n">
         <v>4587</v>
@@ -813,13 +813,13 @@
         </is>
       </c>
       <c r="D13" t="n">
-        <v>205106761.5958301</v>
+        <v>205106761.5958304</v>
       </c>
       <c r="E13" t="n">
         <v>170724820162.3337</v>
       </c>
       <c r="F13" t="n">
-        <v>4758414.451739362</v>
+        <v>4758414.451739367</v>
       </c>
       <c r="G13" t="n">
         <v>43006</v>
@@ -843,13 +843,13 @@
         </is>
       </c>
       <c r="D14" t="n">
-        <v>251799182.9536998</v>
+        <v>251799182.9537001</v>
       </c>
       <c r="E14" t="n">
         <v>210216029160.138</v>
       </c>
       <c r="F14" t="n">
-        <v>5852340.520680402</v>
+        <v>5852340.520680403</v>
       </c>
       <c r="G14" t="n">
         <v>63804</v>
@@ -873,7 +873,7 @@
         </is>
       </c>
       <c r="D15" t="n">
-        <v>11870308.2292655</v>
+        <v>11870308.22926551</v>
       </c>
       <c r="E15" t="n">
         <v>10026485766.11506</v>
@@ -903,13 +903,13 @@
         </is>
       </c>
       <c r="D16" t="n">
-        <v>494975.9084090959</v>
+        <v>494975.908409096</v>
       </c>
       <c r="E16" t="n">
-        <v>412310895.6668767</v>
+        <v>412310895.6668766</v>
       </c>
       <c r="F16" t="n">
-        <v>11484.85305662544</v>
+        <v>11484.85305662545</v>
       </c>
       <c r="G16" t="n">
         <v>337</v>
@@ -933,10 +933,10 @@
         </is>
       </c>
       <c r="D17" t="n">
-        <v>52721017.04956283</v>
+        <v>52721017.04956282</v>
       </c>
       <c r="E17" t="n">
-        <v>43985416320.07995</v>
+        <v>43985416320.07998</v>
       </c>
       <c r="F17" t="n">
         <v>1226084.069182385</v>
@@ -963,10 +963,10 @@
         </is>
       </c>
       <c r="D18" t="n">
-        <v>91738591.03588867</v>
+        <v>91738591.03588861</v>
       </c>
       <c r="E18" t="n">
-        <v>81039326079.31822</v>
+        <v>81039326079.31821</v>
       </c>
       <c r="F18" t="n">
         <v>2225840.824616437</v>
@@ -993,13 +993,13 @@
         </is>
       </c>
       <c r="D19" t="n">
-        <v>2525171.179992207</v>
+        <v>2525171.179992206</v>
       </c>
       <c r="E19" t="n">
         <v>2132935729.531038</v>
       </c>
       <c r="F19" t="n">
-        <v>59290.48899468255</v>
+        <v>59290.48899468256</v>
       </c>
       <c r="G19" t="n">
         <v>925</v>
@@ -1023,13 +1023,13 @@
         </is>
       </c>
       <c r="D20" t="n">
-        <v>9963548.853430858</v>
+        <v>9963548.85343086</v>
       </c>
       <c r="E20" t="n">
-        <v>8392401550.127663</v>
+        <v>8392401550.127668</v>
       </c>
       <c r="F20" t="n">
-        <v>233186.3624315747</v>
+        <v>233186.362431575</v>
       </c>
       <c r="G20" t="n">
         <v>3264</v>
@@ -1053,7 +1053,7 @@
         </is>
       </c>
       <c r="D21" t="n">
-        <v>52508139.09462881</v>
+        <v>52508139.0946288</v>
       </c>
       <c r="E21" t="n">
         <v>43255098221.54024</v>
@@ -1083,13 +1083,13 @@
         </is>
       </c>
       <c r="D22" t="n">
-        <v>36691217.34793752</v>
+        <v>36691217.34793753</v>
       </c>
       <c r="E22" t="n">
-        <v>30473044580.54581</v>
+        <v>30473044580.54578</v>
       </c>
       <c r="F22" t="n">
-        <v>848214.4046380481</v>
+        <v>848214.4046380478</v>
       </c>
       <c r="G22" t="n">
         <v>14785</v>
@@ -1113,13 +1113,13 @@
         </is>
       </c>
       <c r="D23" t="n">
-        <v>34285358.26433827</v>
+        <v>34285358.26433826</v>
       </c>
       <c r="E23" t="n">
-        <v>28563078117.44635</v>
+        <v>28563078117.44634</v>
       </c>
       <c r="F23" t="n">
-        <v>794698.5048573811</v>
+        <v>794698.5048573806</v>
       </c>
       <c r="G23" t="n">
         <v>8762</v>
@@ -1143,13 +1143,13 @@
         </is>
       </c>
       <c r="D24" t="n">
-        <v>23967006.98026074</v>
+        <v>23967006.98026075</v>
       </c>
       <c r="E24" t="n">
         <v>20503562716.54434</v>
       </c>
       <c r="F24" t="n">
-        <v>568521.2847631535</v>
+        <v>568521.2847631534</v>
       </c>
       <c r="G24" t="n">
         <v>1481</v>
@@ -1173,13 +1173,13 @@
         </is>
       </c>
       <c r="D25" t="n">
-        <v>15364000.6626886</v>
+        <v>15364000.66268861</v>
       </c>
       <c r="E25" t="n">
         <v>12689755966.47028</v>
       </c>
       <c r="F25" t="n">
-        <v>353845.9428119243</v>
+        <v>353845.9428119235</v>
       </c>
       <c r="G25" t="n">
         <v>1700</v>
@@ -1209,7 +1209,7 @@
         <v>1527308548.169326</v>
       </c>
       <c r="F26" t="n">
-        <v>43101.84868506077</v>
+        <v>43101.84868506075</v>
       </c>
       <c r="G26" t="n">
         <v>344</v>
@@ -1233,13 +1233,13 @@
         </is>
       </c>
       <c r="D27" t="n">
-        <v>2395403.278509306</v>
+        <v>2395403.278509304</v>
       </c>
       <c r="E27" t="n">
         <v>2066272067.721378</v>
       </c>
       <c r="F27" t="n">
-        <v>57247.05753823436</v>
+        <v>57247.05753823435</v>
       </c>
       <c r="G27" t="n">
         <v>601</v>
@@ -1263,10 +1263,10 @@
         </is>
       </c>
       <c r="D28" t="n">
-        <v>72875960.01250418</v>
+        <v>72875960.01250419</v>
       </c>
       <c r="E28" t="n">
-        <v>59712846814.3094</v>
+        <v>59712846814.30937</v>
       </c>
       <c r="F28" t="n">
         <v>1662619.216731532</v>
@@ -1293,10 +1293,10 @@
         </is>
       </c>
       <c r="D29" t="n">
-        <v>52218136.03123297</v>
+        <v>52218136.03123294</v>
       </c>
       <c r="E29" t="n">
-        <v>44553962151.117</v>
+        <v>44553962151.11699</v>
       </c>
       <c r="F29" t="n">
         <v>1237211.31349136</v>
@@ -1323,10 +1323,10 @@
         </is>
       </c>
       <c r="D30" t="n">
-        <v>6120142.174316909</v>
+        <v>6120142.174316912</v>
       </c>
       <c r="E30" t="n">
-        <v>5106332778.247774</v>
+        <v>5106332778.247773</v>
       </c>
       <c r="F30" t="n">
         <v>142198.4108820184</v>
@@ -1356,10 +1356,10 @@
         <v>28909538.42255041</v>
       </c>
       <c r="E31" t="n">
-        <v>24566005533.89088</v>
+        <v>24566005533.89089</v>
       </c>
       <c r="F31" t="n">
-        <v>682071.6794349918</v>
+        <v>682071.6794349917</v>
       </c>
       <c r="G31" t="n">
         <v>7468</v>
@@ -1383,10 +1383,10 @@
         </is>
       </c>
       <c r="D32" t="n">
-        <v>80853824.93573737</v>
+        <v>80853824.93573739</v>
       </c>
       <c r="E32" t="n">
-        <v>66928779161.82392</v>
+        <v>66928779161.8239</v>
       </c>
       <c r="F32" t="n">
         <v>1878776.906108669</v>
@@ -1413,10 +1413,10 @@
         </is>
       </c>
       <c r="D33" t="n">
-        <v>2330692.190301179</v>
+        <v>2330692.19030118</v>
       </c>
       <c r="E33" t="n">
-        <v>1951770397.225201</v>
+        <v>1951770397.2252</v>
       </c>
       <c r="F33" t="n">
         <v>54213.14152311482</v>
@@ -1446,7 +1446,7 @@
         <v>56276358.48401083</v>
       </c>
       <c r="E34" t="n">
-        <v>47297437442.88458</v>
+        <v>47297437442.88461</v>
       </c>
       <c r="F34" t="n">
         <v>1314402.4484166</v>
@@ -1473,10 +1473,10 @@
         </is>
       </c>
       <c r="D35" t="n">
-        <v>567854.5605569445</v>
+        <v>567854.560556945</v>
       </c>
       <c r="E35" t="n">
-        <v>484486126.5133661</v>
+        <v>484486126.513366</v>
       </c>
       <c r="F35" t="n">
         <v>13446.09579800181</v>
@@ -1503,13 +1503,13 @@
         </is>
       </c>
       <c r="D36" t="n">
-        <v>47115196.38004861</v>
+        <v>47115196.38004867</v>
       </c>
       <c r="E36" t="n">
         <v>39480664597.43571</v>
       </c>
       <c r="F36" t="n">
-        <v>1098534.592124314</v>
+        <v>1098534.592124315</v>
       </c>
       <c r="G36" t="n">
         <v>17866</v>
@@ -1533,13 +1533,13 @@
         </is>
       </c>
       <c r="D37" t="n">
-        <v>357492186.2775568</v>
+        <v>357492186.2775576</v>
       </c>
       <c r="E37" t="n">
-        <v>298797534342.643</v>
+        <v>298797534342.6429</v>
       </c>
       <c r="F37" t="n">
-        <v>8317031.274379686</v>
+        <v>8317031.274379683</v>
       </c>
       <c r="G37" t="n">
         <v>70420</v>
@@ -1563,13 +1563,13 @@
         </is>
       </c>
       <c r="D38" t="n">
-        <v>85679127.69202723</v>
+        <v>85679127.69202724</v>
       </c>
       <c r="E38" t="n">
         <v>71058890817.55539</v>
       </c>
       <c r="F38" t="n">
-        <v>1977719.927269286</v>
+        <v>1977719.927269287</v>
       </c>
       <c r="G38" t="n">
         <v>12206</v>
@@ -1593,13 +1593,13 @@
         </is>
       </c>
       <c r="D39" t="n">
-        <v>30217657.20223492</v>
+        <v>30217657.20223491</v>
       </c>
       <c r="E39" t="n">
-        <v>25194614411.85108</v>
+        <v>25194614411.85109</v>
       </c>
       <c r="F39" t="n">
-        <v>701956.4696915724</v>
+        <v>701956.4696915722</v>
       </c>
       <c r="G39" t="n">
         <v>11623</v>
@@ -1653,13 +1653,13 @@
         </is>
       </c>
       <c r="D41" t="n">
-        <v>340062698.3191185</v>
+        <v>340062698.3191183</v>
       </c>
       <c r="E41" t="n">
-        <v>283935173099.2924</v>
+        <v>283935173099.2922</v>
       </c>
       <c r="F41" t="n">
-        <v>7901732.124620393</v>
+        <v>7901732.124620392</v>
       </c>
       <c r="G41" t="n">
         <v>73525</v>
@@ -1683,13 +1683,13 @@
         </is>
       </c>
       <c r="D42" t="n">
-        <v>1420587.427262706</v>
+        <v>1420587.427262705</v>
       </c>
       <c r="E42" t="n">
         <v>1190084574.358965</v>
       </c>
       <c r="F42" t="n">
-        <v>33071.8731070272</v>
+        <v>33071.87310702722</v>
       </c>
       <c r="G42" t="n">
         <v>452</v>
@@ -1713,13 +1713,13 @@
         </is>
       </c>
       <c r="D43" t="n">
-        <v>3949812.565978677</v>
+        <v>3949812.565978678</v>
       </c>
       <c r="E43" t="n">
-        <v>3313440008.66914</v>
+        <v>3313440008.669139</v>
       </c>
       <c r="F43" t="n">
-        <v>92201.0416973571</v>
+        <v>92201.04169735714</v>
       </c>
       <c r="G43" t="n">
         <v>1050</v>
@@ -1743,10 +1743,10 @@
         </is>
       </c>
       <c r="D44" t="n">
-        <v>71650113.97637287</v>
+        <v>71650113.97637284</v>
       </c>
       <c r="E44" t="n">
-        <v>59206117085.99327</v>
+        <v>59206117085.99329</v>
       </c>
       <c r="F44" t="n">
         <v>1654104.675245431</v>
@@ -1773,13 +1773,13 @@
         </is>
       </c>
       <c r="D45" t="n">
-        <v>2480573.616309847</v>
+        <v>2480573.616309846</v>
       </c>
       <c r="E45" t="n">
         <v>2068309207.113719</v>
       </c>
       <c r="F45" t="n">
-        <v>57521.68634497989</v>
+        <v>57521.6863449799</v>
       </c>
       <c r="G45" t="n">
         <v>1068</v>
@@ -1806,10 +1806,10 @@
         <v>1058134.663958397</v>
       </c>
       <c r="E46" t="n">
-        <v>881569872.7257911</v>
+        <v>881569872.7257912</v>
       </c>
       <c r="F46" t="n">
-        <v>24480.12477207714</v>
+        <v>24480.12477207713</v>
       </c>
       <c r="G46" t="n">
         <v>332</v>
@@ -1839,7 +1839,7 @@
         <v>37954515358.42428</v>
       </c>
       <c r="F47" t="n">
-        <v>1055617.927062331</v>
+        <v>1055617.927062332</v>
       </c>
       <c r="G47" t="n">
         <v>9278</v>
@@ -1869,7 +1869,7 @@
         <v>111957821896.7086</v>
       </c>
       <c r="F48" t="n">
-        <v>3113119.599287472</v>
+        <v>3113119.599287473</v>
       </c>
       <c r="G48" t="n">
         <v>29660</v>
@@ -1893,13 +1893,13 @@
         </is>
       </c>
       <c r="D49" t="n">
-        <v>2994580.950294237</v>
+        <v>2994580.950294234</v>
       </c>
       <c r="E49" t="n">
-        <v>2506731631.994281</v>
+        <v>2506731631.994278</v>
       </c>
       <c r="F49" t="n">
-        <v>69649.67652717035</v>
+        <v>69649.67652717039</v>
       </c>
       <c r="G49" t="n">
         <v>1415</v>
@@ -1923,13 +1923,13 @@
         </is>
       </c>
       <c r="D50" t="n">
-        <v>120466135.0154177</v>
+        <v>120466135.0154176</v>
       </c>
       <c r="E50" t="n">
-        <v>100624577281.6628</v>
+        <v>100624577281.6629</v>
       </c>
       <c r="F50" t="n">
-        <v>2800065.41317059</v>
+        <v>2800065.413170587</v>
       </c>
       <c r="G50" t="n">
         <v>29966</v>
@@ -1953,13 +1953,13 @@
         </is>
       </c>
       <c r="D51" t="n">
-        <v>413670.7442199462</v>
+        <v>413670.7442199463</v>
       </c>
       <c r="E51" t="n">
-        <v>347390119.7075499</v>
+        <v>347390119.70755</v>
       </c>
       <c r="F51" t="n">
-        <v>9672.069104297225</v>
+        <v>9672.069104297219</v>
       </c>
       <c r="G51" t="n">
         <v>225</v>
@@ -1983,13 +1983,13 @@
         </is>
       </c>
       <c r="D52" t="n">
-        <v>96439051.3074723</v>
+        <v>96439051.30747224</v>
       </c>
       <c r="E52" t="n">
         <v>80942396536.40842</v>
       </c>
       <c r="F52" t="n">
-        <v>2253075.974834648</v>
+        <v>2253075.974834647</v>
       </c>
       <c r="G52" t="n">
         <v>22761</v>
@@ -2019,7 +2019,7 @@
         <v>2415701361.33981</v>
       </c>
       <c r="F53" t="n">
-        <v>67141.40969618602</v>
+        <v>67141.40969618603</v>
       </c>
       <c r="G53" t="n">
         <v>891</v>
@@ -2046,10 +2046,10 @@
         <v>11115696.26345669</v>
       </c>
       <c r="E54" t="n">
-        <v>9226436401.465487</v>
+        <v>9226436401.465488</v>
       </c>
       <c r="F54" t="n">
-        <v>256684.5361098767</v>
+        <v>256684.5361098768</v>
       </c>
       <c r="G54" t="n">
         <v>1401</v>
@@ -2076,10 +2076,10 @@
         <v>209760063.8688557</v>
       </c>
       <c r="E55" t="n">
-        <v>174889438480.5923</v>
+        <v>174889438480.5924</v>
       </c>
       <c r="F55" t="n">
-        <v>4873551.146942781</v>
+        <v>4873551.146942782</v>
       </c>
       <c r="G55" t="n">
         <v>50945</v>
@@ -2109,7 +2109,7 @@
         <v>22163070347.56158</v>
       </c>
       <c r="F56" t="n">
-        <v>613670.3541360424</v>
+        <v>613670.3541360423</v>
       </c>
       <c r="G56" t="n">
         <v>929</v>
@@ -2133,10 +2133,10 @@
         </is>
       </c>
       <c r="D57" t="n">
-        <v>46176821.02082905</v>
+        <v>46176821.02082907</v>
       </c>
       <c r="E57" t="n">
-        <v>38505347253.23792</v>
+        <v>38505347253.23791</v>
       </c>
       <c r="F57" t="n">
         <v>1073491.227564266</v>
@@ -2163,13 +2163,13 @@
         </is>
       </c>
       <c r="D58" t="n">
-        <v>12759064.30416485</v>
+        <v>12759064.30416487</v>
       </c>
       <c r="E58" t="n">
-        <v>10565650187.29556</v>
+        <v>10565650187.29555</v>
       </c>
       <c r="F58" t="n">
-        <v>294771.6626018512</v>
+        <v>294771.6626018515</v>
       </c>
       <c r="G58" t="n">
         <v>3009</v>
@@ -2193,10 +2193,10 @@
         </is>
       </c>
       <c r="D59" t="n">
-        <v>45538039.30874518</v>
+        <v>45538039.30874515</v>
       </c>
       <c r="E59" t="n">
-        <v>37814807100.00154</v>
+        <v>37814807100.00153</v>
       </c>
       <c r="F59" t="n">
         <v>1049088.262274222</v>
@@ -2226,10 +2226,10 @@
         <v>11151570.20154089</v>
       </c>
       <c r="E60" t="n">
-        <v>9316333186.476517</v>
+        <v>9316333186.476511</v>
       </c>
       <c r="F60" t="n">
-        <v>259150.0712940934</v>
+        <v>259150.0712940932</v>
       </c>
       <c r="G60" t="n">
         <v>5198</v>
@@ -2253,13 +2253,13 @@
         </is>
       </c>
       <c r="D61" t="n">
-        <v>41148852.70435169</v>
+        <v>41148852.70435167</v>
       </c>
       <c r="E61" t="n">
-        <v>34529259910.13265</v>
+        <v>34529259910.13268</v>
       </c>
       <c r="F61" t="n">
-        <v>959583.2070805322</v>
+        <v>959583.2070805326</v>
       </c>
       <c r="G61" t="n">
         <v>11589</v>
@@ -2283,13 +2283,13 @@
         </is>
       </c>
       <c r="D62" t="n">
-        <v>212398296.8753042</v>
+        <v>212398296.8753038</v>
       </c>
       <c r="E62" t="n">
-        <v>177597832800.8744</v>
+        <v>177597832800.8743</v>
       </c>
       <c r="F62" t="n">
-        <v>4941783.725445349</v>
+        <v>4941783.725445353</v>
       </c>
       <c r="G62" t="n">
         <v>50226</v>
@@ -2316,10 +2316,10 @@
         <v>199545622.8739138</v>
       </c>
       <c r="E63" t="n">
-        <v>165522351401.3824</v>
+        <v>165522351401.3821</v>
       </c>
       <c r="F63" t="n">
-        <v>4619274.48829016</v>
+        <v>4619274.488290163</v>
       </c>
       <c r="G63" t="n">
         <v>50915</v>
@@ -2343,13 +2343,13 @@
         </is>
       </c>
       <c r="D64" t="n">
-        <v>648547.2715135284</v>
+        <v>648547.2715135281</v>
       </c>
       <c r="E64" t="n">
         <v>535800571.3971754</v>
       </c>
       <c r="F64" t="n">
-        <v>14932.33337335807</v>
+        <v>14932.33337335806</v>
       </c>
       <c r="G64" t="n">
         <v>468</v>
@@ -2373,13 +2373,13 @@
         </is>
       </c>
       <c r="D65" t="n">
-        <v>3827344.637616131</v>
+        <v>3827344.637616133</v>
       </c>
       <c r="E65" t="n">
         <v>3201217157.450672</v>
       </c>
       <c r="F65" t="n">
-        <v>89043.29451076745</v>
+        <v>89043.29451076739</v>
       </c>
       <c r="G65" t="n">
         <v>1506</v>
@@ -2403,13 +2403,13 @@
         </is>
       </c>
       <c r="D66" t="n">
-        <v>118537465.7527871</v>
+        <v>118537465.7527872</v>
       </c>
       <c r="E66" t="n">
         <v>98946830988.556</v>
       </c>
       <c r="F66" t="n">
-        <v>2754681.77970799</v>
+        <v>2754681.779707988</v>
       </c>
       <c r="G66" t="n">
         <v>33662</v>
@@ -2436,10 +2436,10 @@
         <v>535232.3020515819</v>
       </c>
       <c r="E67" t="n">
-        <v>450378498.8130659</v>
+        <v>450378498.813066</v>
       </c>
       <c r="F67" t="n">
-        <v>12492.08731702589</v>
+        <v>12492.0873170259</v>
       </c>
       <c r="G67" t="n">
         <v>320</v>
@@ -2463,13 +2463,13 @@
         </is>
       </c>
       <c r="D68" t="n">
-        <v>1937128.154539606</v>
+        <v>1937128.154539607</v>
       </c>
       <c r="E68" t="n">
         <v>1609586700.433693</v>
       </c>
       <c r="F68" t="n">
-        <v>44808.09377541535</v>
+        <v>44808.0937754154</v>
       </c>
       <c r="G68" t="n">
         <v>751</v>
@@ -2493,13 +2493,13 @@
         </is>
       </c>
       <c r="D69" t="n">
-        <v>22748566.80603402</v>
+        <v>22748566.80603403</v>
       </c>
       <c r="E69" t="n">
         <v>18901498789.40987</v>
       </c>
       <c r="F69" t="n">
-        <v>526814.4678034105</v>
+        <v>526814.4678034106</v>
       </c>
       <c r="G69" t="n">
         <v>6312</v>
@@ -2523,13 +2523,13 @@
         </is>
       </c>
       <c r="D70" t="n">
-        <v>76997480.74837053</v>
+        <v>76997480.74837029</v>
       </c>
       <c r="E70" t="n">
-        <v>64163284186.26353</v>
+        <v>64163284186.26357</v>
       </c>
       <c r="F70" t="n">
-        <v>1785413.008767212</v>
+        <v>1785413.008767213</v>
       </c>
       <c r="G70" t="n">
         <v>22809</v>
@@ -2553,13 +2553,13 @@
         </is>
       </c>
       <c r="D71" t="n">
-        <v>115660938.0749669</v>
+        <v>115660938.074967</v>
       </c>
       <c r="E71" t="n">
-        <v>94270719379.04428</v>
+        <v>94270719379.04434</v>
       </c>
       <c r="F71" t="n">
-        <v>2624781.04080397</v>
+        <v>2624781.040803971</v>
       </c>
       <c r="G71" t="n">
         <v>1485</v>
@@ -2583,7 +2583,7 @@
         </is>
       </c>
       <c r="D72" t="n">
-        <v>3729076.927355961</v>
+        <v>3729076.927355962</v>
       </c>
       <c r="E72" t="n">
         <v>3182315326.086373</v>
@@ -2619,7 +2619,7 @@
         <v>15487133212.3417</v>
       </c>
       <c r="F73" t="n">
-        <v>430643.0193201298</v>
+        <v>430643.0193201297</v>
       </c>
       <c r="G73" t="n">
         <v>9259</v>
@@ -2643,10 +2643,10 @@
         </is>
       </c>
       <c r="D74" t="n">
-        <v>78780592.23354155</v>
+        <v>78780592.23354153</v>
       </c>
       <c r="E74" t="n">
-        <v>68387467721.37945</v>
+        <v>68387467721.37946</v>
       </c>
       <c r="F74" t="n">
         <v>1890359.769936774</v>
@@ -2673,13 +2673,13 @@
         </is>
       </c>
       <c r="D75" t="n">
-        <v>31371839.11540125</v>
+        <v>31371839.11540124</v>
       </c>
       <c r="E75" t="n">
         <v>26366342423.53283</v>
       </c>
       <c r="F75" t="n">
-        <v>734109.9689866373</v>
+        <v>734109.9689866372</v>
       </c>
       <c r="G75" t="n">
         <v>7499</v>
@@ -2703,13 +2703,13 @@
         </is>
       </c>
       <c r="D76" t="n">
-        <v>74806803.35066856</v>
+        <v>74806803.35066859</v>
       </c>
       <c r="E76" t="n">
-        <v>62086703911.82234</v>
+        <v>62086703911.82242</v>
       </c>
       <c r="F76" t="n">
-        <v>1730578.354390216</v>
+        <v>1730578.354390209</v>
       </c>
       <c r="G76" t="n">
         <v>19602</v>
@@ -2733,13 +2733,13 @@
         </is>
       </c>
       <c r="D77" t="n">
-        <v>854837.5795743995</v>
+        <v>854837.579574399</v>
       </c>
       <c r="E77" t="n">
-        <v>701498269.1297921</v>
+        <v>701498269.1297925</v>
       </c>
       <c r="F77" t="n">
-        <v>19583.50213372596</v>
+        <v>19583.50213372595</v>
       </c>
       <c r="G77" t="n">
         <v>160</v>
@@ -2763,13 +2763,13 @@
         </is>
       </c>
       <c r="D78" t="n">
-        <v>28494413.16688111</v>
+        <v>28494413.1668811</v>
       </c>
       <c r="E78" t="n">
-        <v>23816346818.02434</v>
+        <v>23816346818.02435</v>
       </c>
       <c r="F78" t="n">
-        <v>663528.3709464342</v>
+        <v>663528.370946434</v>
       </c>
       <c r="G78" t="n">
         <v>9797</v>
@@ -2796,7 +2796,7 @@
         <v>768827.6125303237</v>
       </c>
       <c r="E79" t="n">
-        <v>639275078.101216</v>
+        <v>639275078.1012162</v>
       </c>
       <c r="F79" t="n">
         <v>17831.31801429973</v>
@@ -2823,13 +2823,13 @@
         </is>
       </c>
       <c r="D80" t="n">
-        <v>275712700.7003271</v>
+        <v>275712700.700327</v>
       </c>
       <c r="E80" t="n">
         <v>229884896127.4651</v>
       </c>
       <c r="F80" t="n">
-        <v>6413464.57767286</v>
+        <v>6413464.577672858</v>
       </c>
       <c r="G80" t="n">
         <v>65583</v>
@@ -2853,13 +2853,13 @@
         </is>
       </c>
       <c r="D81" t="n">
-        <v>123205293.6489912</v>
+        <v>123205293.6489913</v>
       </c>
       <c r="E81" t="n">
         <v>103392852367.6661</v>
       </c>
       <c r="F81" t="n">
-        <v>2860454.94610891</v>
+        <v>2860454.946108908</v>
       </c>
       <c r="G81" t="n">
         <v>1242</v>
@@ -2883,10 +2883,10 @@
         </is>
       </c>
       <c r="D82" t="n">
-        <v>6293528.489209347</v>
+        <v>6293528.489209346</v>
       </c>
       <c r="E82" t="n">
-        <v>5299536033.971366</v>
+        <v>5299536033.971365</v>
       </c>
       <c r="F82" t="n">
         <v>147524.1748241123</v>
@@ -2913,13 +2913,13 @@
         </is>
       </c>
       <c r="D83" t="n">
-        <v>80270683.31188142</v>
+        <v>80270683.31188138</v>
       </c>
       <c r="E83" t="n">
-        <v>67032421190.68655</v>
+        <v>67032421190.68652</v>
       </c>
       <c r="F83" t="n">
-        <v>1863552.724494704</v>
+        <v>1863552.724494705</v>
       </c>
       <c r="G83" t="n">
         <v>14255</v>
@@ -2943,13 +2943,13 @@
         </is>
       </c>
       <c r="D84" t="n">
-        <v>3566083.537784517</v>
+        <v>3566083.537784518</v>
       </c>
       <c r="E84" t="n">
         <v>2979136857.855999</v>
       </c>
       <c r="F84" t="n">
-        <v>82875.3209474816</v>
+        <v>82875.32094748158</v>
       </c>
       <c r="G84" t="n">
         <v>1081</v>
@@ -2979,7 +2979,7 @@
         <v>143730998061.9495</v>
       </c>
       <c r="F85" t="n">
-        <v>3996778.617263735</v>
+        <v>3996778.617263731</v>
       </c>
       <c r="G85" t="n">
         <v>52478</v>
@@ -3006,10 +3006,10 @@
         <v>2917256209.440227</v>
       </c>
       <c r="E86" t="n">
-        <v>2420840222758.181</v>
+        <v>2420840222758.179</v>
       </c>
       <c r="F86" t="n">
-        <v>67439122.9451874</v>
+        <v>67439122.94518742</v>
       </c>
       <c r="G86" t="n">
         <v>195266</v>
@@ -3033,13 +3033,13 @@
         </is>
       </c>
       <c r="D87" t="n">
-        <v>80325511.4316873</v>
+        <v>80325511.43168731</v>
       </c>
       <c r="E87" t="n">
-        <v>67375533457.16412</v>
+        <v>67375533457.16415</v>
       </c>
       <c r="F87" t="n">
-        <v>1871732.682566267</v>
+        <v>1871732.682566268</v>
       </c>
       <c r="G87" t="n">
         <v>14471</v>
@@ -3069,7 +3069,7 @@
         <v>890259220101.5947</v>
       </c>
       <c r="F88" t="n">
-        <v>24775392.36973763</v>
+        <v>24775392.36973764</v>
       </c>
       <c r="G88" t="n">
         <v>94051</v>
@@ -3093,13 +3093,13 @@
         </is>
       </c>
       <c r="D89" t="n">
-        <v>2389776999.254036</v>
+        <v>2389776999.254038</v>
       </c>
       <c r="E89" t="n">
-        <v>1995829778728.002</v>
+        <v>1995829778728.003</v>
       </c>
       <c r="F89" t="n">
-        <v>55581277.59502076</v>
+        <v>55581277.59502075</v>
       </c>
       <c r="G89" t="n">
         <v>123002</v>
@@ -3123,13 +3123,13 @@
         </is>
       </c>
       <c r="D90" t="n">
-        <v>528675043.8712052</v>
+        <v>528675043.8712048</v>
       </c>
       <c r="E90" t="n">
-        <v>439689985213.753</v>
+        <v>439689985213.7524</v>
       </c>
       <c r="F90" t="n">
-        <v>12297852.68143745</v>
+        <v>12297852.68143746</v>
       </c>
       <c r="G90" t="n">
         <v>63944</v>
@@ -3156,10 +3156,10 @@
         <v>697221013.2083693</v>
       </c>
       <c r="E91" t="n">
-        <v>574261303287.5353</v>
+        <v>574261303287.5354</v>
       </c>
       <c r="F91" t="n">
-        <v>16029467.82296856</v>
+        <v>16029467.82296857</v>
       </c>
       <c r="G91" t="n">
         <v>7554</v>
@@ -3186,10 +3186,10 @@
         <v>34609444.72622526</v>
       </c>
       <c r="E92" t="n">
-        <v>28518803529.31038</v>
+        <v>28518803529.31037</v>
       </c>
       <c r="F92" t="n">
-        <v>796631.6906681118</v>
+        <v>796631.6906681122</v>
       </c>
       <c r="G92" t="n">
         <v>2957</v>
@@ -3219,7 +3219,7 @@
         <v>89350743131.55698</v>
       </c>
       <c r="F93" t="n">
-        <v>2482708.735199223</v>
+        <v>2482708.735199221</v>
       </c>
       <c r="G93" t="n">
         <v>28062</v>
@@ -3243,10 +3243,10 @@
         </is>
       </c>
       <c r="D94" t="n">
-        <v>1784479.663923215</v>
+        <v>1784479.663923214</v>
       </c>
       <c r="E94" t="n">
-        <v>1494286717.650224</v>
+        <v>1494286717.650223</v>
       </c>
       <c r="F94" t="n">
         <v>41506.39762253487</v>
@@ -3333,7 +3333,7 @@
         </is>
       </c>
       <c r="D97" t="n">
-        <v>32660450.19740819</v>
+        <v>32660450.1974082</v>
       </c>
       <c r="E97" t="n">
         <v>27563855750.46714</v>
@@ -3366,10 +3366,10 @@
         <v>136709407.4514824</v>
       </c>
       <c r="E98" t="n">
-        <v>114068426013.5349</v>
+        <v>114068426013.535</v>
       </c>
       <c r="F98" t="n">
-        <v>3176114.185560541</v>
+        <v>3176114.18556054</v>
       </c>
       <c r="G98" t="n">
         <v>43656</v>
@@ -3393,10 +3393,10 @@
         </is>
       </c>
       <c r="D99" t="n">
-        <v>654613.2604004714</v>
+        <v>654613.260400471</v>
       </c>
       <c r="E99" t="n">
-        <v>555737190.7161075</v>
+        <v>555737190.7161074</v>
       </c>
       <c r="F99" t="n">
         <v>15414.45181971</v>
@@ -3426,10 +3426,10 @@
         <v>1094140.767058617</v>
       </c>
       <c r="E100" t="n">
-        <v>929692293.8628387</v>
+        <v>929692293.8628389</v>
       </c>
       <c r="F100" t="n">
-        <v>25798.36519395662</v>
+        <v>25798.36519395663</v>
       </c>
       <c r="G100" t="n">
         <v>416</v>
@@ -3453,13 +3453,13 @@
         </is>
       </c>
       <c r="D101" t="n">
-        <v>20359298.82018407</v>
+        <v>20359298.82018408</v>
       </c>
       <c r="E101" t="n">
-        <v>17341104650.55721</v>
+        <v>17341104650.5572</v>
       </c>
       <c r="F101" t="n">
-        <v>482193.9663938576</v>
+        <v>482193.9663938575</v>
       </c>
       <c r="G101" t="n">
         <v>836</v>
@@ -3486,10 +3486,10 @@
         <v>2903187.278975379</v>
       </c>
       <c r="E102" t="n">
-        <v>2472549305.845934</v>
+        <v>2472549305.845933</v>
       </c>
       <c r="F102" t="n">
-        <v>68378.71535572656</v>
+        <v>68378.71535572653</v>
       </c>
       <c r="G102" t="n">
         <v>709</v>
@@ -3513,13 +3513,13 @@
         </is>
       </c>
       <c r="D103" t="n">
-        <v>54428951.11142073</v>
+        <v>54428951.11142085</v>
       </c>
       <c r="E103" t="n">
-        <v>45670255329.09625</v>
+        <v>45670255329.09623</v>
       </c>
       <c r="F103" t="n">
-        <v>1270383.00295112</v>
+        <v>1270383.002951121</v>
       </c>
       <c r="G103" t="n">
         <v>13127</v>
@@ -3543,13 +3543,13 @@
         </is>
       </c>
       <c r="D104" t="n">
-        <v>69084107.85523304</v>
+        <v>69084107.85523303</v>
       </c>
       <c r="E104" t="n">
-        <v>58026929805.83485</v>
+        <v>58026929805.83482</v>
       </c>
       <c r="F104" t="n">
-        <v>1614479.163622733</v>
+        <v>1614479.163622735</v>
       </c>
       <c r="G104" t="n">
         <v>9549</v>
@@ -3573,13 +3573,13 @@
         </is>
       </c>
       <c r="D105" t="n">
-        <v>43236223.61105492</v>
+        <v>43236223.61105493</v>
       </c>
       <c r="E105" t="n">
         <v>36152337262.27254</v>
       </c>
       <c r="F105" t="n">
-        <v>1003375.525671833</v>
+        <v>1003375.525671834</v>
       </c>
       <c r="G105" t="n">
         <v>8040</v>
@@ -3603,10 +3603,10 @@
         </is>
       </c>
       <c r="D106" t="n">
-        <v>10835548.39357416</v>
+        <v>10835548.39357415</v>
       </c>
       <c r="E106" t="n">
-        <v>9084737929.485752</v>
+        <v>9084737929.485748</v>
       </c>
       <c r="F106" t="n">
         <v>252747.8416477506</v>
@@ -3639,7 +3639,7 @@
         <v>200594092766.6549</v>
       </c>
       <c r="F107" t="n">
-        <v>5571895.822994118</v>
+        <v>5571895.822994121</v>
       </c>
       <c r="G107" t="n">
         <v>22917</v>
@@ -3669,7 +3669,7 @@
         <v>14206515836.26536</v>
       </c>
       <c r="F108" t="n">
-        <v>394937.223663417</v>
+        <v>394937.2236634169</v>
       </c>
       <c r="G108" t="n">
         <v>3263</v>
@@ -3696,10 +3696,10 @@
         <v>122870149.5509931</v>
       </c>
       <c r="E109" t="n">
-        <v>102846041891.1931</v>
+        <v>102846041891.1934</v>
       </c>
       <c r="F109" t="n">
-        <v>2863054.64540446</v>
+        <v>2863054.645404453</v>
       </c>
       <c r="G109" t="n">
         <v>25807</v>
@@ -3723,13 +3723,13 @@
         </is>
       </c>
       <c r="D110" t="n">
-        <v>16769530.38298286</v>
+        <v>16769530.38298285</v>
       </c>
       <c r="E110" t="n">
         <v>13960519596.35183</v>
       </c>
       <c r="F110" t="n">
-        <v>389624.3414204617</v>
+        <v>389624.3414204618</v>
       </c>
       <c r="G110" t="n">
         <v>2744</v>
@@ -3753,13 +3753,13 @@
         </is>
       </c>
       <c r="D111" t="n">
-        <v>360775243.0513492</v>
+        <v>360775243.0513493</v>
       </c>
       <c r="E111" t="n">
-        <v>299194016952.4321</v>
+        <v>299194016952.4323</v>
       </c>
       <c r="F111" t="n">
-        <v>8339722.64331224</v>
+        <v>8339722.643312238</v>
       </c>
       <c r="G111" t="n">
         <v>66367</v>
@@ -3783,13 +3783,13 @@
         </is>
       </c>
       <c r="D112" t="n">
-        <v>326396505.9896716</v>
+        <v>326396505.9896717</v>
       </c>
       <c r="E112" t="n">
-        <v>272825620843.8128</v>
+        <v>272825620843.8127</v>
       </c>
       <c r="F112" t="n">
-        <v>7594994.788875364</v>
+        <v>7594994.788875362</v>
       </c>
       <c r="G112" t="n">
         <v>66993</v>
@@ -3849,7 +3849,7 @@
         <v>28769334463.46619</v>
       </c>
       <c r="F114" t="n">
-        <v>872689.8672431011</v>
+        <v>872689.8672431009</v>
       </c>
       <c r="G114" t="n">
         <v>7375</v>
@@ -3873,13 +3873,13 @@
         </is>
       </c>
       <c r="D115" t="n">
-        <v>710701.5735204211</v>
+        <v>710701.5735204213</v>
       </c>
       <c r="E115" t="n">
         <v>616077307.3500706</v>
       </c>
       <c r="F115" t="n">
-        <v>18766.18171234422</v>
+        <v>18766.18171234423</v>
       </c>
       <c r="G115" t="n">
         <v>415</v>
@@ -3903,13 +3903,13 @@
         </is>
       </c>
       <c r="D116" t="n">
-        <v>6874801.682265432</v>
+        <v>6874801.682265433</v>
       </c>
       <c r="E116" t="n">
         <v>5982539182.686913</v>
       </c>
       <c r="F116" t="n">
-        <v>181677.5324824289</v>
+        <v>181677.5324824287</v>
       </c>
       <c r="G116" t="n">
         <v>3467</v>
@@ -3963,13 +3963,13 @@
         </is>
       </c>
       <c r="D118" t="n">
-        <v>67159379.69239694</v>
+        <v>67159379.69239691</v>
       </c>
       <c r="E118" t="n">
-        <v>58846642883.09242</v>
+        <v>58846642883.09241</v>
       </c>
       <c r="F118" t="n">
-        <v>1782763.932256107</v>
+        <v>1782763.932256106</v>
       </c>
       <c r="G118" t="n">
         <v>8568</v>
@@ -3996,7 +3996,7 @@
         <v>41656558.22845215</v>
       </c>
       <c r="E119" t="n">
-        <v>35101226764.02649</v>
+        <v>35101226764.02648</v>
       </c>
       <c r="F119" t="n">
         <v>1091285.080324018</v>
@@ -4026,10 +4026,10 @@
         <v>77908320.54239939</v>
       </c>
       <c r="E120" t="n">
-        <v>67055907735.38192</v>
+        <v>67055907735.38196</v>
       </c>
       <c r="F120" t="n">
-        <v>2059572.84946377</v>
+        <v>2059572.849463773</v>
       </c>
       <c r="G120" t="n">
         <v>13479</v>
@@ -4053,10 +4053,10 @@
         </is>
       </c>
       <c r="D121" t="n">
-        <v>50188940.66446244</v>
+        <v>50188940.66446242</v>
       </c>
       <c r="E121" t="n">
-        <v>43076301299.14088</v>
+        <v>43076301299.14089</v>
       </c>
       <c r="F121" t="n">
         <v>1321819.257414042</v>
@@ -4083,13 +4083,13 @@
         </is>
       </c>
       <c r="D122" t="n">
-        <v>70758599.38973534</v>
+        <v>70758599.38973536</v>
       </c>
       <c r="E122" t="n">
-        <v>61810249042.65454</v>
+        <v>61810249042.65456</v>
       </c>
       <c r="F122" t="n">
-        <v>1872931.247505296</v>
+        <v>1872931.247505297</v>
       </c>
       <c r="G122" t="n">
         <v>14846</v>
@@ -4113,13 +4113,13 @@
         </is>
       </c>
       <c r="D123" t="n">
-        <v>526514.0195496344</v>
+        <v>526514.0195496342</v>
       </c>
       <c r="E123" t="n">
         <v>477564506.3738856</v>
       </c>
       <c r="F123" t="n">
-        <v>14212.11584043224</v>
+        <v>14212.11584043223</v>
       </c>
       <c r="G123" t="n">
         <v>595</v>
@@ -4143,13 +4143,13 @@
         </is>
       </c>
       <c r="D124" t="n">
-        <v>12257783.69057348</v>
+        <v>12257783.69057349</v>
       </c>
       <c r="E124" t="n">
-        <v>10614373719.47994</v>
+        <v>10614373719.47993</v>
       </c>
       <c r="F124" t="n">
-        <v>323843.095540137</v>
+        <v>323843.0955401368</v>
       </c>
       <c r="G124" t="n">
         <v>3807</v>
@@ -4173,13 +4173,13 @@
         </is>
       </c>
       <c r="D125" t="n">
-        <v>167588174.6531513</v>
+        <v>167588174.6531512</v>
       </c>
       <c r="E125" t="n">
-        <v>145819193828.2275</v>
+        <v>145819193828.2274</v>
       </c>
       <c r="F125" t="n">
-        <v>4443939.613301172</v>
+        <v>4443939.613301169</v>
       </c>
       <c r="G125" t="n">
         <v>39132</v>
@@ -4206,10 +4206,10 @@
         <v>202344234.1082084</v>
       </c>
       <c r="E126" t="n">
-        <v>176759934467.3819</v>
+        <v>176759934467.382</v>
       </c>
       <c r="F126" t="n">
-        <v>5359483.304230302</v>
+        <v>5359483.304230295</v>
       </c>
       <c r="G126" t="n">
         <v>62415</v>
@@ -4233,10 +4233,10 @@
         </is>
       </c>
       <c r="D127" t="n">
-        <v>6691172.429902971</v>
+        <v>6691172.429902968</v>
       </c>
       <c r="E127" t="n">
-        <v>5919793101.499161</v>
+        <v>5919793101.499163</v>
       </c>
       <c r="F127" t="n">
         <v>178444.9640117613</v>
@@ -4263,13 +4263,13 @@
         </is>
       </c>
       <c r="D128" t="n">
-        <v>3113683.980026728</v>
+        <v>3113683.980026726</v>
       </c>
       <c r="E128" t="n">
-        <v>2667079613.835338</v>
+        <v>2667079613.83534</v>
       </c>
       <c r="F128" t="n">
-        <v>81649.92966293292</v>
+        <v>81649.9296629329</v>
       </c>
       <c r="G128" t="n">
         <v>343</v>
@@ -4293,13 +4293,13 @@
         </is>
       </c>
       <c r="D129" t="n">
-        <v>51561600.394953</v>
+        <v>51561600.39495303</v>
       </c>
       <c r="E129" t="n">
-        <v>44207440124.09162</v>
+        <v>44207440124.09158</v>
       </c>
       <c r="F129" t="n">
-        <v>1349890.713777267</v>
+        <v>1349890.713777268</v>
       </c>
       <c r="G129" t="n">
         <v>10372</v>
@@ -4323,7 +4323,7 @@
         </is>
       </c>
       <c r="D130" t="n">
-        <v>49776060.71459825</v>
+        <v>49776060.71459826</v>
       </c>
       <c r="E130" t="n">
         <v>42881082809.80994</v>
@@ -4353,7 +4353,7 @@
         </is>
       </c>
       <c r="D131" t="n">
-        <v>2131544.458758038</v>
+        <v>2131544.458758037</v>
       </c>
       <c r="E131" t="n">
         <v>1896434995.662169</v>
@@ -4383,7 +4383,7 @@
         </is>
       </c>
       <c r="D132" t="n">
-        <v>13603139.76146509</v>
+        <v>13603139.7614651</v>
       </c>
       <c r="E132" t="n">
         <v>12182237495.68213</v>
@@ -4413,7 +4413,7 @@
         </is>
       </c>
       <c r="D133" t="n">
-        <v>15178392.93773502</v>
+        <v>15178392.937735</v>
       </c>
       <c r="E133" t="n">
         <v>13446097784.74991</v>
@@ -4443,13 +4443,13 @@
         </is>
       </c>
       <c r="D134" t="n">
-        <v>27795436.39813892</v>
+        <v>27795436.39813901</v>
       </c>
       <c r="E134" t="n">
         <v>24412745526.62838</v>
       </c>
       <c r="F134" t="n">
-        <v>739429.9857332351</v>
+        <v>739429.9857332358</v>
       </c>
       <c r="G134" t="n">
         <v>12024</v>
@@ -4473,13 +4473,13 @@
         </is>
       </c>
       <c r="D135" t="n">
-        <v>31336286.68588776</v>
+        <v>31336286.68588778</v>
       </c>
       <c r="E135" t="n">
-        <v>27639548628.81014</v>
+        <v>27639548628.81015</v>
       </c>
       <c r="F135" t="n">
-        <v>835325.5484630408</v>
+        <v>835325.548463041</v>
       </c>
       <c r="G135" t="n">
         <v>7580</v>
@@ -4503,13 +4503,13 @@
         </is>
       </c>
       <c r="D136" t="n">
-        <v>152702487.9470846</v>
+        <v>152702487.9470845</v>
       </c>
       <c r="E136" t="n">
-        <v>131598655558.611</v>
+        <v>131598655558.6109</v>
       </c>
       <c r="F136" t="n">
-        <v>4043426.862018499</v>
+        <v>4043426.862018502</v>
       </c>
       <c r="G136" t="n">
         <v>1676</v>
@@ -4533,13 +4533,13 @@
         </is>
       </c>
       <c r="D137" t="n">
-        <v>8762907.739684444</v>
+        <v>8762907.739684448</v>
       </c>
       <c r="E137" t="n">
         <v>7758556674.854376</v>
       </c>
       <c r="F137" t="n">
-        <v>232643.2866542686</v>
+        <v>232643.2866542684</v>
       </c>
       <c r="G137" t="n">
         <v>1568</v>
@@ -4563,10 +4563,10 @@
         </is>
       </c>
       <c r="D138" t="n">
-        <v>387892.0284583171</v>
+        <v>387892.0284583172</v>
       </c>
       <c r="E138" t="n">
-        <v>343559755.5548731</v>
+        <v>343559755.554873</v>
       </c>
       <c r="F138" t="n">
         <v>10304.74718001448</v>
@@ -4596,7 +4596,7 @@
         <v>1141855.068036881</v>
       </c>
       <c r="E139" t="n">
-        <v>987256743.6839055</v>
+        <v>987256743.6839056</v>
       </c>
       <c r="F139" t="n">
         <v>30205.08250428116</v>
@@ -4623,13 +4623,13 @@
         </is>
       </c>
       <c r="D140" t="n">
-        <v>40292318.05305228</v>
+        <v>40292318.05305227</v>
       </c>
       <c r="E140" t="n">
         <v>34837284710.04025</v>
       </c>
       <c r="F140" t="n">
-        <v>1063627.296876333</v>
+        <v>1063627.296876334</v>
       </c>
       <c r="G140" t="n">
         <v>12187</v>
@@ -4653,10 +4653,10 @@
         </is>
       </c>
       <c r="D141" t="n">
-        <v>51009503.57818478</v>
+        <v>51009503.5781848</v>
       </c>
       <c r="E141" t="n">
-        <v>44668820977.47053</v>
+        <v>44668820977.47054</v>
       </c>
       <c r="F141" t="n">
         <v>1356899.431238746</v>
@@ -4683,10 +4683,10 @@
         </is>
       </c>
       <c r="D142" t="n">
-        <v>5845186.301155093</v>
+        <v>5845186.301155091</v>
       </c>
       <c r="E142" t="n">
-        <v>5119005435.376383</v>
+        <v>5119005435.376384</v>
       </c>
       <c r="F142" t="n">
         <v>155057.6395018318</v>
@@ -4713,13 +4713,13 @@
         </is>
       </c>
       <c r="D143" t="n">
-        <v>21455534.82763781</v>
+        <v>21455534.82763782</v>
       </c>
       <c r="E143" t="n">
-        <v>18938162189.86214</v>
+        <v>18938162189.86213</v>
       </c>
       <c r="F143" t="n">
-        <v>570045.1477604391</v>
+        <v>570045.1477604393</v>
       </c>
       <c r="G143" t="n">
         <v>7299</v>
@@ -4743,13 +4743,13 @@
         </is>
       </c>
       <c r="D144" t="n">
-        <v>30225485.28794665</v>
+        <v>30225485.28794664</v>
       </c>
       <c r="E144" t="n">
         <v>26156450383.5216</v>
       </c>
       <c r="F144" t="n">
-        <v>801571.3382594704</v>
+        <v>801571.3382594702</v>
       </c>
       <c r="G144" t="n">
         <v>1632</v>
@@ -4773,7 +4773,7 @@
         </is>
       </c>
       <c r="D145" t="n">
-        <v>512573.962804489</v>
+        <v>512573.9628044889</v>
       </c>
       <c r="E145" t="n">
         <v>454154719.1583012</v>
@@ -4806,10 +4806,10 @@
         <v>29192760.96468332</v>
       </c>
       <c r="E146" t="n">
-        <v>25395189919.08704</v>
+        <v>25395189919.08703</v>
       </c>
       <c r="F146" t="n">
-        <v>773241.7808059959</v>
+        <v>773241.7808059964</v>
       </c>
       <c r="G146" t="n">
         <v>9663</v>
@@ -4833,10 +4833,10 @@
         </is>
       </c>
       <c r="D147" t="n">
-        <v>288153.0072041912</v>
+        <v>288153.0072041913</v>
       </c>
       <c r="E147" t="n">
-        <v>259221026.3650102</v>
+        <v>259221026.3650101</v>
       </c>
       <c r="F147" t="n">
         <v>7726.687497293841</v>
@@ -4896,10 +4896,10 @@
         <v>298725166.9743878</v>
       </c>
       <c r="E149" t="n">
-        <v>260408138617.5942</v>
+        <v>260408138617.594</v>
       </c>
       <c r="F149" t="n">
-        <v>7921722.977568181</v>
+        <v>7921722.977568176</v>
       </c>
       <c r="G149" t="n">
         <v>67457</v>
@@ -4923,10 +4923,10 @@
         </is>
       </c>
       <c r="D150" t="n">
-        <v>53393463.80524924</v>
+        <v>53393463.80524926</v>
       </c>
       <c r="E150" t="n">
-        <v>46869874606.70302</v>
+        <v>46869874606.70301</v>
       </c>
       <c r="F150" t="n">
         <v>1416736.655941303</v>
@@ -4953,13 +4953,13 @@
         </is>
       </c>
       <c r="D151" t="n">
-        <v>22503472.81004543</v>
+        <v>22503472.81004542</v>
       </c>
       <c r="E151" t="n">
-        <v>19794379371.47837</v>
+        <v>19794379371.47836</v>
       </c>
       <c r="F151" t="n">
-        <v>598426.8571609582</v>
+        <v>598426.8571609583</v>
       </c>
       <c r="G151" t="n">
         <v>11632</v>
@@ -4983,7 +4983,7 @@
         </is>
       </c>
       <c r="D152" t="n">
-        <v>184544594.639917</v>
+        <v>184544594.6399171</v>
       </c>
       <c r="E152" t="n">
         <v>158937066571.7104</v>
@@ -5013,7 +5013,7 @@
         </is>
       </c>
       <c r="D153" t="n">
-        <v>234615139.4562356</v>
+        <v>234615139.4562357</v>
       </c>
       <c r="E153" t="n">
         <v>205438169464.2921</v>
@@ -5043,7 +5043,7 @@
         </is>
       </c>
       <c r="D154" t="n">
-        <v>1145362.547420053</v>
+        <v>1145362.547420054</v>
       </c>
       <c r="E154" t="n">
         <v>1026603028.711061</v>
@@ -5079,7 +5079,7 @@
         <v>2119407634.815138</v>
       </c>
       <c r="F155" t="n">
-        <v>64326.78943543147</v>
+        <v>64326.78943543148</v>
       </c>
       <c r="G155" t="n">
         <v>685</v>
@@ -5106,10 +5106,10 @@
         <v>111884438.2738182</v>
       </c>
       <c r="E156" t="n">
-        <v>93044380072.86415</v>
+        <v>93044380072.86418</v>
       </c>
       <c r="F156" t="n">
-        <v>2878233.890430296</v>
+        <v>2878233.890430295</v>
       </c>
       <c r="G156" t="n">
         <v>1514</v>
@@ -5136,7 +5136,7 @@
         <v>934460.7940506182</v>
       </c>
       <c r="E157" t="n">
-        <v>848624842.9662023</v>
+        <v>848624842.9662019</v>
       </c>
       <c r="F157" t="n">
         <v>25291.21426216856</v>
@@ -5193,13 +5193,13 @@
         </is>
       </c>
       <c r="D159" t="n">
-        <v>36535755.1624733</v>
+        <v>36535755.16247329</v>
       </c>
       <c r="E159" t="n">
-        <v>32030250146.25706</v>
+        <v>32030250146.25708</v>
       </c>
       <c r="F159" t="n">
-        <v>968080.4893952531</v>
+        <v>968080.4893952536</v>
       </c>
       <c r="G159" t="n">
         <v>8439</v>
@@ -5223,13 +5223,13 @@
         </is>
       </c>
       <c r="D160" t="n">
-        <v>122587182.4811709</v>
+        <v>122587182.481171</v>
       </c>
       <c r="E160" t="n">
-        <v>108801240459.7738</v>
+        <v>108801240459.7739</v>
       </c>
       <c r="F160" t="n">
-        <v>3273149.801801646</v>
+        <v>3273149.801801648</v>
       </c>
       <c r="G160" t="n">
         <v>27852</v>
@@ -5253,10 +5253,10 @@
         </is>
       </c>
       <c r="D161" t="n">
-        <v>2239798.279101386</v>
+        <v>2239798.279101387</v>
       </c>
       <c r="E161" t="n">
-        <v>1971034468.859047</v>
+        <v>1971034468.859048</v>
       </c>
       <c r="F161" t="n">
         <v>59593.94314095753</v>
@@ -5286,7 +5286,7 @@
         <v>105798324.7570809</v>
       </c>
       <c r="E162" t="n">
-        <v>91868419128.5079</v>
+        <v>91868419128.50787</v>
       </c>
       <c r="F162" t="n">
         <v>2799652.219299383</v>
@@ -5319,7 +5319,7 @@
         <v>1133869223.875967</v>
       </c>
       <c r="F163" t="n">
-        <v>33370.53364508587</v>
+        <v>33370.53364508585</v>
       </c>
       <c r="G163" t="n">
         <v>283</v>
@@ -5343,13 +5343,13 @@
         </is>
       </c>
       <c r="D164" t="n">
-        <v>85036783.61023469</v>
+        <v>85036783.61023462</v>
       </c>
       <c r="E164" t="n">
-        <v>73357911728.84802</v>
+        <v>73357911728.84804</v>
       </c>
       <c r="F164" t="n">
-        <v>2243603.506909729</v>
+        <v>2243603.50690973</v>
       </c>
       <c r="G164" t="n">
         <v>22114</v>
@@ -5373,13 +5373,13 @@
         </is>
       </c>
       <c r="D165" t="n">
-        <v>2441618.684916603</v>
+        <v>2441618.684916604</v>
       </c>
       <c r="E165" t="n">
         <v>2185091662.000384</v>
       </c>
       <c r="F165" t="n">
-        <v>65868.57109966149</v>
+        <v>65868.57109966151</v>
       </c>
       <c r="G165" t="n">
         <v>875</v>
@@ -5403,13 +5403,13 @@
         </is>
       </c>
       <c r="D166" t="n">
-        <v>9379165.288931437</v>
+        <v>9379165.288931435</v>
       </c>
       <c r="E166" t="n">
-        <v>8388656244.602973</v>
+        <v>8388656244.60297</v>
       </c>
       <c r="F166" t="n">
-        <v>249753.8356357961</v>
+        <v>249753.835635796</v>
       </c>
       <c r="G166" t="n">
         <v>1620</v>
@@ -5433,13 +5433,13 @@
         </is>
       </c>
       <c r="D167" t="n">
-        <v>155898549.6676878</v>
+        <v>155898549.6676879</v>
       </c>
       <c r="E167" t="n">
         <v>136473885108.0844</v>
       </c>
       <c r="F167" t="n">
-        <v>4136591.983835426</v>
+        <v>4136591.983835427</v>
       </c>
       <c r="G167" t="n">
         <v>46949</v>
@@ -5463,7 +5463,7 @@
         </is>
       </c>
       <c r="D168" t="n">
-        <v>88748160.55327635</v>
+        <v>88748160.55327632</v>
       </c>
       <c r="E168" t="n">
         <v>76631001959.91418</v>
@@ -5493,10 +5493,10 @@
         </is>
       </c>
       <c r="D169" t="n">
-        <v>45119758.12291288</v>
+        <v>45119758.12291286</v>
       </c>
       <c r="E169" t="n">
-        <v>39823003316.18626</v>
+        <v>39823003316.18625</v>
       </c>
       <c r="F169" t="n">
         <v>1200114.50323152</v>
@@ -5523,13 +5523,13 @@
         </is>
       </c>
       <c r="D170" t="n">
-        <v>9545536.458760697</v>
+        <v>9545536.458760696</v>
       </c>
       <c r="E170" t="n">
         <v>8336533797.804822</v>
       </c>
       <c r="F170" t="n">
-        <v>252195.1886726509</v>
+        <v>252195.1886726507</v>
       </c>
       <c r="G170" t="n">
         <v>3006</v>
@@ -5553,13 +5553,13 @@
         </is>
       </c>
       <c r="D171" t="n">
-        <v>71702928.03295134</v>
+        <v>71702928.0329513</v>
       </c>
       <c r="E171" t="n">
-        <v>65641194855.94946</v>
+        <v>65641194855.94948</v>
       </c>
       <c r="F171" t="n">
-        <v>1938690.248983527</v>
+        <v>1938690.248983528</v>
       </c>
       <c r="G171" t="n">
         <v>2379</v>
@@ -5586,10 +5586,10 @@
         <v>9177141.655780507</v>
       </c>
       <c r="E172" t="n">
-        <v>8107877738.486714</v>
+        <v>8107877738.486716</v>
       </c>
       <c r="F172" t="n">
-        <v>244833.7169323673</v>
+        <v>244833.7169323674</v>
       </c>
       <c r="G172" t="n">
         <v>4693</v>
@@ -5643,13 +5643,13 @@
         </is>
       </c>
       <c r="D174" t="n">
-        <v>141739496.8566209</v>
+        <v>141739496.8566208</v>
       </c>
       <c r="E174" t="n">
-        <v>123051851234.1892</v>
+        <v>123051851234.1893</v>
       </c>
       <c r="F174" t="n">
-        <v>3750610.50412173</v>
+        <v>3750610.504121724</v>
       </c>
       <c r="G174" t="n">
         <v>42867</v>
@@ -5673,13 +5673,13 @@
         </is>
       </c>
       <c r="D175" t="n">
-        <v>172382061.137284</v>
+        <v>172382061.1372841</v>
       </c>
       <c r="E175" t="n">
-        <v>149106733651.498</v>
+        <v>149106733651.4979</v>
       </c>
       <c r="F175" t="n">
-        <v>4550610.894700991</v>
+        <v>4550610.894700997</v>
       </c>
       <c r="G175" t="n">
         <v>49983</v>
@@ -5703,13 +5703,13 @@
         </is>
       </c>
       <c r="D176" t="n">
-        <v>1838545.353341679</v>
+        <v>1838545.353341678</v>
       </c>
       <c r="E176" t="n">
         <v>1654256956.019821</v>
       </c>
       <c r="F176" t="n">
-        <v>49222.71897845668</v>
+        <v>49222.71897845666</v>
       </c>
       <c r="G176" t="n">
         <v>417</v>
@@ -5736,10 +5736,10 @@
         <v>3256717.816895179</v>
       </c>
       <c r="E177" t="n">
-        <v>2856936620.085303</v>
+        <v>2856936620.085302</v>
       </c>
       <c r="F177" t="n">
-        <v>86728.39324103376</v>
+        <v>86728.39324103379</v>
       </c>
       <c r="G177" t="n">
         <v>1520</v>
@@ -5763,13 +5763,13 @@
         </is>
       </c>
       <c r="D178" t="n">
-        <v>91506681.3427069</v>
+        <v>91506681.34270687</v>
       </c>
       <c r="E178" t="n">
-        <v>79496032008.23856</v>
+        <v>79496032008.23862</v>
       </c>
       <c r="F178" t="n">
-        <v>2422887.792067335</v>
+        <v>2422887.792067334</v>
       </c>
       <c r="G178" t="n">
         <v>31010</v>
@@ -5793,7 +5793,7 @@
         </is>
       </c>
       <c r="D179" t="n">
-        <v>922005.0638205127</v>
+        <v>922005.063820513</v>
       </c>
       <c r="E179" t="n">
         <v>829745067.9249541</v>
@@ -5823,7 +5823,7 @@
         </is>
       </c>
       <c r="D180" t="n">
-        <v>1226166.042232234</v>
+        <v>1226166.042232233</v>
       </c>
       <c r="E180" t="n">
         <v>1081533328.731198</v>
@@ -5859,7 +5859,7 @@
         <v>17259962627.91117</v>
       </c>
       <c r="F181" t="n">
-        <v>522239.2793969167</v>
+        <v>522239.2793969166</v>
       </c>
       <c r="G181" t="n">
         <v>6004</v>
@@ -5883,13 +5883,13 @@
         </is>
       </c>
       <c r="D182" t="n">
-        <v>54133634.80841435</v>
+        <v>54133634.80841444</v>
       </c>
       <c r="E182" t="n">
         <v>47590001322.35064</v>
       </c>
       <c r="F182" t="n">
-        <v>1439878.599993849</v>
+        <v>1439878.599993848</v>
       </c>
       <c r="G182" t="n">
         <v>19405</v>
@@ -5916,10 +5916,10 @@
         <v>100935711.485358</v>
       </c>
       <c r="E183" t="n">
-        <v>86720594499.11932</v>
+        <v>86720594499.11934</v>
       </c>
       <c r="F183" t="n">
-        <v>2651872.999441817</v>
+        <v>2651872.999441816</v>
       </c>
       <c r="G183" t="n">
         <v>1364</v>
@@ -5976,10 +5976,10 @@
         <v>17113463.91180169</v>
       </c>
       <c r="E185" t="n">
-        <v>15013040527.35411</v>
+        <v>15013040527.35413</v>
       </c>
       <c r="F185" t="n">
-        <v>454962.5045256919</v>
+        <v>454962.504525692</v>
       </c>
       <c r="G185" t="n">
         <v>9610</v>
@@ -6003,7 +6003,7 @@
         </is>
       </c>
       <c r="D186" t="n">
-        <v>59012907.2045265</v>
+        <v>59012907.20452651</v>
       </c>
       <c r="E186" t="n">
         <v>51056256849.08408</v>
@@ -6039,7 +6039,7 @@
         <v>20066683954.22026</v>
       </c>
       <c r="F187" t="n">
-        <v>608074.384312437</v>
+        <v>608074.3843124368</v>
       </c>
       <c r="G187" t="n">
         <v>6539</v>
@@ -6063,7 +6063,7 @@
         </is>
       </c>
       <c r="D188" t="n">
-        <v>42566546.48746517</v>
+        <v>42566546.48746513</v>
       </c>
       <c r="E188" t="n">
         <v>37287949347.68887</v>
@@ -6093,13 +6093,13 @@
         </is>
       </c>
       <c r="D189" t="n">
-        <v>627075.7868480473</v>
+        <v>627075.7868480474</v>
       </c>
       <c r="E189" t="n">
-        <v>563057118.1163071</v>
+        <v>563057118.1163069</v>
       </c>
       <c r="F189" t="n">
-        <v>16785.89108147219</v>
+        <v>16785.8910814722</v>
       </c>
       <c r="G189" t="n">
         <v>109</v>
@@ -6129,7 +6129,7 @@
         <v>22909571285.17046</v>
       </c>
       <c r="F190" t="n">
-        <v>689297.8297485057</v>
+        <v>689297.8297485055</v>
       </c>
       <c r="G190" t="n">
         <v>8649</v>
@@ -6156,10 +6156,10 @@
         <v>483245.5338595731</v>
       </c>
       <c r="E191" t="n">
-        <v>422261047.1978182</v>
+        <v>422261047.197818</v>
       </c>
       <c r="F191" t="n">
-        <v>12797.17327178317</v>
+        <v>12797.17327178318</v>
       </c>
       <c r="G191" t="n">
         <v>496</v>
@@ -6183,10 +6183,10 @@
         </is>
       </c>
       <c r="D192" t="n">
-        <v>194591510.058466</v>
+        <v>194591510.0584659</v>
       </c>
       <c r="E192" t="n">
-        <v>170744465016.6302</v>
+        <v>170744465016.6301</v>
       </c>
       <c r="F192" t="n">
         <v>5170819.162525673</v>
@@ -6213,13 +6213,13 @@
         </is>
       </c>
       <c r="D193" t="n">
-        <v>36049596.12526594</v>
+        <v>36049596.12526596</v>
       </c>
       <c r="E193" t="n">
         <v>31377139607.75195</v>
       </c>
       <c r="F193" t="n">
-        <v>954003.2013326163</v>
+        <v>954003.2013326165</v>
       </c>
       <c r="G193" t="n">
         <v>1420</v>
@@ -6276,10 +6276,10 @@
         <v>82805866.07873154</v>
       </c>
       <c r="E195" t="n">
-        <v>72629007270.93265</v>
+        <v>72629007270.93262</v>
       </c>
       <c r="F195" t="n">
-        <v>2199307.792932808</v>
+        <v>2199307.792932807</v>
       </c>
       <c r="G195" t="n">
         <v>13581</v>
@@ -6303,13 +6303,13 @@
         </is>
       </c>
       <c r="D196" t="n">
-        <v>3022702.540173782</v>
+        <v>3022702.540173781</v>
       </c>
       <c r="E196" t="n">
         <v>2667752654.240418</v>
       </c>
       <c r="F196" t="n">
-        <v>80523.52190361016</v>
+        <v>80523.52190361021</v>
       </c>
       <c r="G196" t="n">
         <v>1236</v>
@@ -6333,13 +6333,13 @@
         </is>
       </c>
       <c r="D197" t="n">
-        <v>134191385.2429575</v>
+        <v>134191385.2429574</v>
       </c>
       <c r="E197" t="n">
-        <v>116374902717.9039</v>
+        <v>116374902717.9038</v>
       </c>
       <c r="F197" t="n">
-        <v>3548258.72803349</v>
+        <v>3548258.728033492</v>
       </c>
       <c r="G197" t="n">
         <v>46872</v>
@@ -6369,7 +6369,7 @@
         <v>2625495739863.608</v>
       </c>
       <c r="F198" t="n">
-        <v>80785730.55555114</v>
+        <v>80785730.55555116</v>
       </c>
       <c r="G198" t="n">
         <v>170272</v>
@@ -6393,13 +6393,13 @@
         </is>
       </c>
       <c r="D199" t="n">
-        <v>26162675.04322941</v>
+        <v>26162675.0432294</v>
       </c>
       <c r="E199" t="n">
-        <v>23513840988.23354</v>
+        <v>23513840988.23353</v>
       </c>
       <c r="F199" t="n">
-        <v>699180.8997297992</v>
+        <v>699180.8997297996</v>
       </c>
       <c r="G199" t="n">
         <v>5424</v>
@@ -6423,7 +6423,7 @@
         </is>
       </c>
       <c r="D200" t="n">
-        <v>732739556.3435209</v>
+        <v>732739556.3435216</v>
       </c>
       <c r="E200" t="n">
         <v>639146086650.6517</v>
@@ -6456,10 +6456,10 @@
         <v>2289302528.297373</v>
       </c>
       <c r="E201" t="n">
-        <v>1949750306973.602</v>
+        <v>1949750306973.601</v>
       </c>
       <c r="F201" t="n">
-        <v>59959915.62653278</v>
+        <v>59959915.62653282</v>
       </c>
       <c r="G201" t="n">
         <v>100942</v>
@@ -6486,10 +6486,10 @@
         <v>374348744.8577887</v>
       </c>
       <c r="E202" t="n">
-        <v>324755253198.7532</v>
+        <v>324755253198.7529</v>
       </c>
       <c r="F202" t="n">
-        <v>9916324.187133921</v>
+        <v>9916324.187133936</v>
       </c>
       <c r="G202" t="n">
         <v>60149</v>
@@ -6513,13 +6513,13 @@
         </is>
       </c>
       <c r="D203" t="n">
-        <v>866689033.8351849</v>
+        <v>866689033.8351853</v>
       </c>
       <c r="E203" t="n">
-        <v>760657149853.3397</v>
+        <v>760657149853.3398</v>
       </c>
       <c r="F203" t="n">
-        <v>23046451.40949858</v>
+        <v>23046451.40949856</v>
       </c>
       <c r="G203" t="n">
         <v>8059</v>
@@ -6543,13 +6543,13 @@
         </is>
       </c>
       <c r="D204" t="n">
-        <v>68355495.42044911</v>
+        <v>68355495.42044903</v>
       </c>
       <c r="E204" t="n">
-        <v>63271104484.38859</v>
+        <v>63271104484.38853</v>
       </c>
       <c r="F204" t="n">
-        <v>1865815.228011515</v>
+        <v>1865815.228011514</v>
       </c>
       <c r="G204" t="n">
         <v>2544</v>
@@ -6573,13 +6573,13 @@
         </is>
       </c>
       <c r="D205" t="n">
-        <v>1250840.334095522</v>
+        <v>1250840.334095523</v>
       </c>
       <c r="E205" t="n">
         <v>1094088227.352716</v>
       </c>
       <c r="F205" t="n">
-        <v>33186.90315836436</v>
+        <v>33186.90315836437</v>
       </c>
       <c r="G205" t="n">
         <v>448</v>
@@ -6609,7 +6609,7 @@
         <v>57246933424.08147</v>
       </c>
       <c r="F206" t="n">
-        <v>1761417.091273216</v>
+        <v>1761417.091273217</v>
       </c>
       <c r="G206" t="n">
         <v>823</v>
@@ -6633,13 +6633,13 @@
         </is>
       </c>
       <c r="D207" t="n">
-        <v>93596795.20972651</v>
+        <v>93596795.20972645</v>
       </c>
       <c r="E207" t="n">
-        <v>82278449116.67323</v>
+        <v>82278449116.67319</v>
       </c>
       <c r="F207" t="n">
-        <v>2488080.512399666</v>
+        <v>2488080.512399667</v>
       </c>
       <c r="G207" t="n">
         <v>42190</v>
@@ -6663,13 +6663,13 @@
         </is>
       </c>
       <c r="D208" t="n">
-        <v>23346642.11882718</v>
+        <v>23346642.11882719</v>
       </c>
       <c r="E208" t="n">
         <v>20542794848.77303</v>
       </c>
       <c r="F208" t="n">
-        <v>619984.3430104766</v>
+        <v>619984.3430104762</v>
       </c>
       <c r="G208" t="n">
         <v>5625</v>
@@ -6693,13 +6693,13 @@
         </is>
       </c>
       <c r="D209" t="n">
-        <v>72441194.59530854</v>
+        <v>72441194.59530857</v>
       </c>
       <c r="E209" t="n">
-        <v>63193365344.36308</v>
+        <v>63193365344.36307</v>
       </c>
       <c r="F209" t="n">
-        <v>1918002.029269865</v>
+        <v>1918002.029269862</v>
       </c>
       <c r="G209" t="n">
         <v>24496</v>
@@ -6726,7 +6726,7 @@
         <v>253319.3409806266</v>
       </c>
       <c r="E210" t="n">
-        <v>219827957.8205878</v>
+        <v>219827957.8205879</v>
       </c>
       <c r="F210" t="n">
         <v>6679.005296085767</v>
@@ -6783,13 +6783,13 @@
         </is>
       </c>
       <c r="D212" t="n">
-        <v>1596802.674130711</v>
+        <v>1596802.674130712</v>
       </c>
       <c r="E212" t="n">
         <v>1396520628.023411</v>
       </c>
       <c r="F212" t="n">
-        <v>42223.2261118468</v>
+        <v>42223.22611184682</v>
       </c>
       <c r="G212" t="n">
         <v>379</v>
@@ -6813,7 +6813,7 @@
         </is>
       </c>
       <c r="D213" t="n">
-        <v>90351912.38580135</v>
+        <v>90351912.38580127</v>
       </c>
       <c r="E213" t="n">
         <v>74450255808.85886</v>
@@ -6873,13 +6873,13 @@
         </is>
       </c>
       <c r="D215" t="n">
-        <v>63352245.17280783</v>
+        <v>63352245.17280784</v>
       </c>
       <c r="E215" t="n">
-        <v>54364843279.28382</v>
+        <v>54364843279.28384</v>
       </c>
       <c r="F215" t="n">
-        <v>1666399.444049633</v>
+        <v>1666399.444049634</v>
       </c>
       <c r="G215" t="n">
         <v>10797</v>
@@ -6906,10 +6906,10 @@
         <v>28614710.2117556</v>
       </c>
       <c r="E216" t="n">
-        <v>25037528375.90477</v>
+        <v>25037528375.90476</v>
       </c>
       <c r="F216" t="n">
-        <v>758078.1380191025</v>
+        <v>758078.1380191026</v>
       </c>
       <c r="G216" t="n">
         <v>6840</v>
@@ -6933,13 +6933,13 @@
         </is>
       </c>
       <c r="D217" t="n">
-        <v>55774368.9307058</v>
+        <v>55774368.93070584</v>
       </c>
       <c r="E217" t="n">
         <v>48795122433.87167</v>
       </c>
       <c r="F217" t="n">
-        <v>1477213.774283428</v>
+        <v>1477213.77428343</v>
       </c>
       <c r="G217" t="n">
         <v>8692</v>
@@ -6963,10 +6963,10 @@
         </is>
       </c>
       <c r="D218" t="n">
-        <v>8599001.821970107</v>
+        <v>8599001.821970109</v>
       </c>
       <c r="E218" t="n">
-        <v>7535640425.283334</v>
+        <v>7535640425.283335</v>
       </c>
       <c r="F218" t="n">
         <v>227866.5694264026</v>
@@ -6996,10 +6996,10 @@
         <v>288942298.7552698</v>
       </c>
       <c r="E219" t="n">
-        <v>248174777271.8875</v>
+        <v>248174777271.8874</v>
       </c>
       <c r="F219" t="n">
-        <v>7601517.327491138</v>
+        <v>7601517.327491141</v>
       </c>
       <c r="G219" t="n">
         <v>20380</v>
@@ -7023,7 +7023,7 @@
         </is>
       </c>
       <c r="D220" t="n">
-        <v>8987647.011521306</v>
+        <v>8987647.011521302</v>
       </c>
       <c r="E220" t="n">
         <v>7946405557.694553</v>
@@ -7053,13 +7053,13 @@
         </is>
       </c>
       <c r="D221" t="n">
-        <v>105925798.7380746</v>
+        <v>105925798.7380748</v>
       </c>
       <c r="E221" t="n">
-        <v>92657333931.53354</v>
+        <v>92657333931.534</v>
       </c>
       <c r="F221" t="n">
-        <v>2811926.25028055</v>
+        <v>2811926.250280549</v>
       </c>
       <c r="G221" t="n">
         <v>25379</v>
@@ -7083,13 +7083,13 @@
         </is>
       </c>
       <c r="D222" t="n">
-        <v>17202792.44964556</v>
+        <v>17202792.44964555</v>
       </c>
       <c r="E222" t="n">
-        <v>15293459152.82519</v>
+        <v>15293459152.82518</v>
       </c>
       <c r="F222" t="n">
-        <v>464594.0752436025</v>
+        <v>464594.0752436024</v>
       </c>
       <c r="G222" t="n">
         <v>2623</v>
@@ -7113,13 +7113,13 @@
         </is>
       </c>
       <c r="D223" t="n">
-        <v>225745082.0110361</v>
+        <v>225745082.011036</v>
       </c>
       <c r="E223" t="n">
         <v>197270847358.6656</v>
       </c>
       <c r="F223" t="n">
-        <v>5985737.055784947</v>
+        <v>5985737.055784949</v>
       </c>
       <c r="G223" t="n">
         <v>58345</v>
@@ -7143,13 +7143,13 @@
         </is>
       </c>
       <c r="D224" t="n">
-        <v>250478015.7520041</v>
+        <v>250478015.7520038</v>
       </c>
       <c r="E224" t="n">
         <v>218269344967.1129</v>
       </c>
       <c r="F224" t="n">
-        <v>6641494.495630589</v>
+        <v>6641494.4956306</v>
       </c>
       <c r="G224" t="n">
         <v>60938</v>
@@ -7173,10 +7173,10 @@
         </is>
       </c>
       <c r="D225" t="n">
-        <v>145684217.3043665</v>
+        <v>145684217.3043666</v>
       </c>
       <c r="E225" t="n">
-        <v>122722381237.9627</v>
+        <v>122722381237.9628</v>
       </c>
       <c r="F225" t="n">
         <v>3780233.668874911</v>
@@ -7203,13 +7203,13 @@
         </is>
       </c>
       <c r="D226" t="n">
-        <v>31862519.3113967</v>
+        <v>31862519.31139667</v>
       </c>
       <c r="E226" t="n">
         <v>23996650849.03104</v>
       </c>
       <c r="F226" t="n">
-        <v>806867.991098347</v>
+        <v>806867.9910983471</v>
       </c>
       <c r="G226" t="n">
         <v>6212</v>
@@ -7233,13 +7233,13 @@
         </is>
       </c>
       <c r="D227" t="n">
-        <v>977463.1188939376</v>
+        <v>977463.1188939374</v>
       </c>
       <c r="E227" t="n">
-        <v>752703886.7749243</v>
+        <v>752703886.7749245</v>
       </c>
       <c r="F227" t="n">
-        <v>25126.98327154579</v>
+        <v>25126.98327154581</v>
       </c>
       <c r="G227" t="n">
         <v>300</v>
@@ -7293,13 +7293,13 @@
         </is>
       </c>
       <c r="D229" t="n">
-        <v>103951.8050724969</v>
+        <v>103951.8050724968</v>
       </c>
       <c r="E229" t="n">
         <v>77679454.73999999</v>
       </c>
       <c r="F229" t="n">
-        <v>2619.285002766343</v>
+        <v>2619.285002766342</v>
       </c>
       <c r="G229" t="n">
         <v>87</v>
@@ -7323,13 +7323,13 @@
         </is>
       </c>
       <c r="D230" t="n">
-        <v>62796055.44291084</v>
+        <v>62796055.44291081</v>
       </c>
       <c r="E230" t="n">
-        <v>47091719272.20409</v>
+        <v>47091719272.20415</v>
       </c>
       <c r="F230" t="n">
-        <v>1585192.317382685</v>
+        <v>1585192.317382686</v>
       </c>
       <c r="G230" t="n">
         <v>6855</v>
@@ -7353,13 +7353,13 @@
         </is>
       </c>
       <c r="D231" t="n">
-        <v>192757875.1052921</v>
+        <v>192757875.1052919</v>
       </c>
       <c r="E231" t="n">
         <v>146265226796.4437</v>
       </c>
       <c r="F231" t="n">
-        <v>4889004.993740452</v>
+        <v>4889004.993740454</v>
       </c>
       <c r="G231" t="n">
         <v>1098</v>
@@ -7383,13 +7383,13 @@
         </is>
       </c>
       <c r="D232" t="n">
-        <v>115556529.1467825</v>
+        <v>115556529.1467828</v>
       </c>
       <c r="E232" t="n">
-        <v>86228957281.48404</v>
+        <v>86228957281.48401</v>
       </c>
       <c r="F232" t="n">
-        <v>2906440.376576537</v>
+        <v>2906440.376576546</v>
       </c>
       <c r="G232" t="n">
         <v>15419</v>
@@ -7413,13 +7413,13 @@
         </is>
       </c>
       <c r="D233" t="n">
-        <v>329671595.9755181</v>
+        <v>329671595.9755179</v>
       </c>
       <c r="E233" t="n">
         <v>244475173597.7556</v>
       </c>
       <c r="F233" t="n">
-        <v>8286835.496757583</v>
+        <v>8286835.496757585</v>
       </c>
       <c r="G233" t="n">
         <v>2225</v>
@@ -7446,7 +7446,7 @@
         <v>70251431.69206958</v>
       </c>
       <c r="E234" t="n">
-        <v>52803119428.34777</v>
+        <v>52803119428.34774</v>
       </c>
       <c r="F234" t="n">
         <v>1775705.350069739</v>
@@ -7473,13 +7473,13 @@
         </is>
       </c>
       <c r="D235" t="n">
-        <v>1901694.625802628</v>
+        <v>1901694.625802625</v>
       </c>
       <c r="E235" t="n">
         <v>1395653528.681727</v>
       </c>
       <c r="F235" t="n">
-        <v>47073.12521678207</v>
+        <v>47073.12521678204</v>
       </c>
       <c r="G235" t="n">
         <v>422</v>
@@ -7503,13 +7503,13 @@
         </is>
       </c>
       <c r="D236" t="n">
-        <v>8269515.823290442</v>
+        <v>8269515.823290456</v>
       </c>
       <c r="E236" t="n">
         <v>6256028313.547626</v>
       </c>
       <c r="F236" t="n">
-        <v>209899.2023186324</v>
+        <v>209899.2023186322</v>
       </c>
       <c r="G236" t="n">
         <v>2512</v>
@@ -7533,13 +7533,13 @@
         </is>
       </c>
       <c r="D237" t="n">
-        <v>182859594.9397833</v>
+        <v>182859594.9397832</v>
       </c>
       <c r="E237" t="n">
-        <v>136661072051.1828</v>
+        <v>136661072051.1827</v>
       </c>
       <c r="F237" t="n">
-        <v>4606667.082416999</v>
+        <v>4606667.08241701</v>
       </c>
       <c r="G237" t="n">
         <v>39080</v>
@@ -7563,13 +7563,13 @@
         </is>
       </c>
       <c r="D238" t="n">
-        <v>208554021.2631379</v>
+        <v>208554021.2631381</v>
       </c>
       <c r="E238" t="n">
         <v>157054195137.3817</v>
       </c>
       <c r="F238" t="n">
-        <v>5282465.849343374</v>
+        <v>5282465.849343372</v>
       </c>
       <c r="G238" t="n">
         <v>53618</v>
@@ -7593,10 +7593,10 @@
         </is>
       </c>
       <c r="D239" t="n">
-        <v>6752126.386595062</v>
+        <v>6752126.386595057</v>
       </c>
       <c r="E239" t="n">
-        <v>5079065494.38719</v>
+        <v>5079065494.387194</v>
       </c>
       <c r="F239" t="n">
         <v>170646.4881368614</v>
@@ -7626,10 +7626,10 @@
         <v>1230358.567517363</v>
       </c>
       <c r="E240" t="n">
-        <v>950485508.2410246</v>
+        <v>950485508.2410249</v>
       </c>
       <c r="F240" t="n">
-        <v>31760.52477455747</v>
+        <v>31760.52477455746</v>
       </c>
       <c r="G240" t="n">
         <v>288</v>
@@ -7656,10 +7656,10 @@
         <v>40179201.97957928</v>
       </c>
       <c r="E241" t="n">
-        <v>30505765000.37809</v>
+        <v>30505765000.3781</v>
       </c>
       <c r="F241" t="n">
-        <v>1023030.435824528</v>
+        <v>1023030.435824527</v>
       </c>
       <c r="G241" t="n">
         <v>8282</v>
@@ -7683,10 +7683,10 @@
         </is>
       </c>
       <c r="D242" t="n">
-        <v>73890318.55277063</v>
+        <v>73890318.5527706</v>
       </c>
       <c r="E242" t="n">
-        <v>54555937177.87874</v>
+        <v>54555937177.87875</v>
       </c>
       <c r="F242" t="n">
         <v>1839179.101175095</v>
@@ -7713,13 +7713,13 @@
         </is>
       </c>
       <c r="D243" t="n">
-        <v>273097.9581904122</v>
+        <v>273097.9581904123</v>
       </c>
       <c r="E243" t="n">
         <v>204413214.8086082</v>
       </c>
       <c r="F243" t="n">
-        <v>6879.893232558256</v>
+        <v>6879.893232558255</v>
       </c>
       <c r="G243" t="n">
         <v>77</v>
@@ -7743,13 +7743,13 @@
         </is>
       </c>
       <c r="D244" t="n">
-        <v>6783734.338989171</v>
+        <v>6783734.338989168</v>
       </c>
       <c r="E244" t="n">
-        <v>5082464388.164809</v>
+        <v>5082464388.164811</v>
       </c>
       <c r="F244" t="n">
-        <v>171070.5785424989</v>
+        <v>171070.578542499</v>
       </c>
       <c r="G244" t="n">
         <v>3141</v>
@@ -7773,13 +7773,13 @@
         </is>
       </c>
       <c r="D245" t="n">
-        <v>23668286.41602092</v>
+        <v>23668286.41602091</v>
       </c>
       <c r="E245" t="n">
-        <v>17742513833.14741</v>
+        <v>17742513833.14743</v>
       </c>
       <c r="F245" t="n">
-        <v>595572.4213999109</v>
+        <v>595572.4213999111</v>
       </c>
       <c r="G245" t="n">
         <v>2617</v>
@@ -7803,13 +7803,13 @@
         </is>
       </c>
       <c r="D246" t="n">
-        <v>36547964.20117464</v>
+        <v>36547964.20117462</v>
       </c>
       <c r="E246" t="n">
         <v>27318495393.80622</v>
       </c>
       <c r="F246" t="n">
-        <v>920002.0786265328</v>
+        <v>920002.0786265333</v>
       </c>
       <c r="G246" t="n">
         <v>10969</v>
@@ -7833,13 +7833,13 @@
         </is>
       </c>
       <c r="D247" t="n">
-        <v>39389622.97321832</v>
+        <v>39389622.97321831</v>
       </c>
       <c r="E247" t="n">
-        <v>29690917214.86665</v>
+        <v>29690917214.86664</v>
       </c>
       <c r="F247" t="n">
-        <v>997996.5322460835</v>
+        <v>997996.532246083</v>
       </c>
       <c r="G247" t="n">
         <v>6166</v>
@@ -7869,7 +7869,7 @@
         <v>45874154464.2596</v>
       </c>
       <c r="F248" t="n">
-        <v>1535310.105123557</v>
+        <v>1535310.105123558</v>
       </c>
       <c r="G248" t="n">
         <v>1530</v>
@@ -7896,10 +7896,10 @@
         <v>9032504.886778209</v>
       </c>
       <c r="E249" t="n">
-        <v>7103275381.136807</v>
+        <v>7103275381.136808</v>
       </c>
       <c r="F249" t="n">
-        <v>235983.3553340797</v>
+        <v>235983.3553340798</v>
       </c>
       <c r="G249" t="n">
         <v>1161</v>
@@ -7923,10 +7923,10 @@
         </is>
       </c>
       <c r="D250" t="n">
-        <v>566577.2545041484</v>
+        <v>566577.2545041485</v>
       </c>
       <c r="E250" t="n">
-        <v>440597990.9135512</v>
+        <v>440597990.9135513</v>
       </c>
       <c r="F250" t="n">
         <v>14648.11345321844</v>
@@ -7953,10 +7953,10 @@
         </is>
       </c>
       <c r="D251" t="n">
-        <v>1258661.83082493</v>
+        <v>1258661.830824931</v>
       </c>
       <c r="E251" t="n">
-        <v>941283531.8848336</v>
+        <v>941283531.8848332</v>
       </c>
       <c r="F251" t="n">
         <v>31692.73935614167</v>
@@ -7983,13 +7983,13 @@
         </is>
       </c>
       <c r="D252" t="n">
-        <v>46868397.51728484</v>
+        <v>46868397.5172848</v>
       </c>
       <c r="E252" t="n">
         <v>34887469745.12026</v>
       </c>
       <c r="F252" t="n">
-        <v>1176909.493562494</v>
+        <v>1176909.493562493</v>
       </c>
       <c r="G252" t="n">
         <v>12168</v>
@@ -8013,13 +8013,13 @@
         </is>
       </c>
       <c r="D253" t="n">
-        <v>45842230.52923071</v>
+        <v>45842230.52923076</v>
       </c>
       <c r="E253" t="n">
-        <v>34493761108.89758</v>
+        <v>34493761108.89755</v>
       </c>
       <c r="F253" t="n">
-        <v>1161174.525705983</v>
+        <v>1161174.525705984</v>
       </c>
       <c r="G253" t="n">
         <v>10791</v>
@@ -8043,13 +8043,13 @@
         </is>
       </c>
       <c r="D254" t="n">
-        <v>5685763.90553051</v>
+        <v>5685763.905530504</v>
       </c>
       <c r="E254" t="n">
-        <v>4269892007.741314</v>
+        <v>4269892007.741317</v>
       </c>
       <c r="F254" t="n">
-        <v>143554.413955619</v>
+        <v>143554.4139556194</v>
       </c>
       <c r="G254" t="n">
         <v>2582</v>
@@ -8103,13 +8103,13 @@
         </is>
       </c>
       <c r="D256" t="n">
-        <v>98408480.50071947</v>
+        <v>98408480.50071944</v>
       </c>
       <c r="E256" t="n">
-        <v>72660943846.35413</v>
+        <v>72660943846.35411</v>
       </c>
       <c r="F256" t="n">
-        <v>2456099.632416021</v>
+        <v>2456099.632416022</v>
       </c>
       <c r="G256" t="n">
         <v>1597</v>
@@ -8163,13 +8163,13 @@
         </is>
       </c>
       <c r="D258" t="n">
-        <v>34134065.60315827</v>
+        <v>34134065.6031583</v>
       </c>
       <c r="E258" t="n">
         <v>25913603036.07952</v>
       </c>
       <c r="F258" t="n">
-        <v>870558.0812341245</v>
+        <v>870558.081234125</v>
       </c>
       <c r="G258" t="n">
         <v>9746</v>
@@ -8199,7 +8199,7 @@
         <v>198315438.8633666</v>
       </c>
       <c r="F259" t="n">
-        <v>6612.713862629067</v>
+        <v>6612.713862629071</v>
       </c>
       <c r="G259" t="n">
         <v>132</v>
@@ -8223,13 +8223,13 @@
         </is>
       </c>
       <c r="D260" t="n">
-        <v>38812534.00005432</v>
+        <v>38812534.00005427</v>
       </c>
       <c r="E260" t="n">
-        <v>29104102428.31553</v>
+        <v>29104102428.31552</v>
       </c>
       <c r="F260" t="n">
-        <v>979289.1125451515</v>
+        <v>979289.1125451529</v>
       </c>
       <c r="G260" t="n">
         <v>12595</v>
@@ -8253,13 +8253,13 @@
         </is>
       </c>
       <c r="D261" t="n">
-        <v>321982101.2586353</v>
+        <v>321982101.2586355</v>
       </c>
       <c r="E261" t="n">
-        <v>239997829550.8156</v>
+        <v>239997829550.8154</v>
       </c>
       <c r="F261" t="n">
-        <v>8090712.346272925</v>
+        <v>8090712.346272927</v>
       </c>
       <c r="G261" t="n">
         <v>64947</v>
@@ -8283,10 +8283,10 @@
         </is>
       </c>
       <c r="D262" t="n">
-        <v>56198733.79919769</v>
+        <v>56198733.79919767</v>
       </c>
       <c r="E262" t="n">
-        <v>42178606595.93551</v>
+        <v>42178606595.9355</v>
       </c>
       <c r="F262" t="n">
         <v>1419674.272518239</v>
@@ -8313,13 +8313,13 @@
         </is>
       </c>
       <c r="D263" t="n">
-        <v>23605661.05662574</v>
+        <v>23605661.05662576</v>
       </c>
       <c r="E263" t="n">
-        <v>17789854564.62149</v>
+        <v>17789854564.62148</v>
       </c>
       <c r="F263" t="n">
-        <v>597337.1702366241</v>
+        <v>597337.1702366224</v>
       </c>
       <c r="G263" t="n">
         <v>12503</v>
@@ -8343,13 +8343,13 @@
         </is>
       </c>
       <c r="D264" t="n">
-        <v>278121883.0573131</v>
+        <v>278121883.057313</v>
       </c>
       <c r="E264" t="n">
-        <v>213356494040.1413</v>
+        <v>213356494040.1412</v>
       </c>
       <c r="F264" t="n">
-        <v>7149112.736308254</v>
+        <v>7149112.736308252</v>
       </c>
       <c r="G264" t="n">
         <v>2033</v>
@@ -8373,13 +8373,13 @@
         </is>
       </c>
       <c r="D265" t="n">
-        <v>281044373.4677522</v>
+        <v>281044373.4677521</v>
       </c>
       <c r="E265" t="n">
-        <v>208885105383.7912</v>
+        <v>208885105383.791</v>
       </c>
       <c r="F265" t="n">
-        <v>7037355.084439324</v>
+        <v>7037355.084439319</v>
       </c>
       <c r="G265" t="n">
         <v>58509</v>
@@ -8406,10 +8406,10 @@
         <v>1907800.358994878</v>
       </c>
       <c r="E266" t="n">
-        <v>1455524216.71895</v>
+        <v>1455524216.718951</v>
       </c>
       <c r="F266" t="n">
-        <v>48596.6785084617</v>
+        <v>48596.67850846169</v>
       </c>
       <c r="G266" t="n">
         <v>432</v>
@@ -8439,7 +8439,7 @@
         <v>342220075.9685841</v>
       </c>
       <c r="F267" t="n">
-        <v>11445.82020894983</v>
+        <v>11445.82020894984</v>
       </c>
       <c r="G267" t="n">
         <v>105</v>
@@ -8463,13 +8463,13 @@
         </is>
       </c>
       <c r="D268" t="n">
-        <v>27704946.77621411</v>
+        <v>27704946.77621408</v>
       </c>
       <c r="E268" t="n">
-        <v>20466701208.20314</v>
+        <v>20466701208.20315</v>
       </c>
       <c r="F268" t="n">
-        <v>691227.2232214821</v>
+        <v>691227.223221482</v>
       </c>
       <c r="G268" t="n">
         <v>1381</v>
@@ -8493,10 +8493,10 @@
         </is>
       </c>
       <c r="D269" t="n">
-        <v>757140.806597462</v>
+        <v>757140.8065974623</v>
       </c>
       <c r="E269" t="n">
-        <v>568055043.1057727</v>
+        <v>568055043.1057726</v>
       </c>
       <c r="F269" t="n">
         <v>19105.15463222886</v>
@@ -8523,13 +8523,13 @@
         </is>
       </c>
       <c r="D270" t="n">
-        <v>1201914.927455134</v>
+        <v>1201914.927455135</v>
       </c>
       <c r="E270" t="n">
-        <v>924175394.0734203</v>
+        <v>924175394.0734206</v>
       </c>
       <c r="F270" t="n">
-        <v>30918.36158240118</v>
+        <v>30918.3615824012</v>
       </c>
       <c r="G270" t="n">
         <v>199</v>
@@ -8553,7 +8553,7 @@
         </is>
       </c>
       <c r="D271" t="n">
-        <v>49300173.93918505</v>
+        <v>49300173.939185</v>
       </c>
       <c r="E271" t="n">
         <v>37268748083.55228</v>
@@ -8586,10 +8586,10 @@
         <v>103003052.708211</v>
       </c>
       <c r="E272" t="n">
-        <v>77169714138.52708</v>
+        <v>77169714138.52705</v>
       </c>
       <c r="F272" t="n">
-        <v>2601525.203811702</v>
+        <v>2601525.203811703</v>
       </c>
       <c r="G272" t="n">
         <v>24344</v>
@@ -8616,10 +8616,10 @@
         <v>2784011.374986758</v>
       </c>
       <c r="E273" t="n">
-        <v>2077620846.4642</v>
+        <v>2077620846.464201</v>
       </c>
       <c r="F273" t="n">
-        <v>69950.73619697211</v>
+        <v>69950.73619697205</v>
       </c>
       <c r="G273" t="n">
         <v>1463</v>
@@ -8643,13 +8643,13 @@
         </is>
       </c>
       <c r="D274" t="n">
-        <v>117603273.2503934</v>
+        <v>117603273.2503935</v>
       </c>
       <c r="E274" t="n">
-        <v>87365972106.20244</v>
+        <v>87365972106.20242</v>
       </c>
       <c r="F274" t="n">
-        <v>2949166.444838098</v>
+        <v>2949166.444838096</v>
       </c>
       <c r="G274" t="n">
         <v>27399</v>
@@ -8676,10 +8676,10 @@
         <v>1009918.146069754</v>
       </c>
       <c r="E275" t="n">
-        <v>764666976.0013242</v>
+        <v>764666976.0013239</v>
       </c>
       <c r="F275" t="n">
-        <v>25610.7253011056</v>
+        <v>25610.72530110559</v>
       </c>
       <c r="G275" t="n">
         <v>210</v>
@@ -8703,10 +8703,10 @@
         </is>
       </c>
       <c r="D276" t="n">
-        <v>89124137.73193249</v>
+        <v>89124137.73193252</v>
       </c>
       <c r="E276" t="n">
-        <v>66048990542.73093</v>
+        <v>66048990542.73092</v>
       </c>
       <c r="F276" t="n">
         <v>2230153.94306701</v>
@@ -8733,13 +8733,13 @@
         </is>
       </c>
       <c r="D277" t="n">
-        <v>2739889.256819723</v>
+        <v>2739889.256819724</v>
       </c>
       <c r="E277" t="n">
         <v>2063954502.796068</v>
       </c>
       <c r="F277" t="n">
-        <v>69294.66127263456</v>
+        <v>69294.66127263449</v>
       </c>
       <c r="G277" t="n">
         <v>1006</v>
@@ -8763,10 +8763,10 @@
         </is>
       </c>
       <c r="D278" t="n">
-        <v>4252049.539239701</v>
+        <v>4252049.539239698</v>
       </c>
       <c r="E278" t="n">
-        <v>3231369489.051355</v>
+        <v>3231369489.051353</v>
       </c>
       <c r="F278" t="n">
         <v>108257.7209904047</v>
@@ -8793,13 +8793,13 @@
         </is>
       </c>
       <c r="D279" t="n">
-        <v>154018193.6247682</v>
+        <v>154018193.6247683</v>
       </c>
       <c r="E279" t="n">
         <v>115564062145.198</v>
       </c>
       <c r="F279" t="n">
-        <v>3887834.645865225</v>
+        <v>3887834.645865223</v>
       </c>
       <c r="G279" t="n">
         <v>40572</v>
@@ -8823,10 +8823,10 @@
         </is>
       </c>
       <c r="D280" t="n">
-        <v>39874016.38968956</v>
+        <v>39874016.38968958</v>
       </c>
       <c r="E280" t="n">
-        <v>29610796298.24539</v>
+        <v>29610796298.24538</v>
       </c>
       <c r="F280" t="n">
         <v>1003128.293206669</v>
@@ -8853,10 +8853,10 @@
         </is>
       </c>
       <c r="D281" t="n">
-        <v>59016078.66376578</v>
+        <v>59016078.66376577</v>
       </c>
       <c r="E281" t="n">
-        <v>44203752380.44099</v>
+        <v>44203752380.44102</v>
       </c>
       <c r="F281" t="n">
         <v>1488054.112141155</v>
@@ -8883,13 +8883,13 @@
         </is>
       </c>
       <c r="D282" t="n">
-        <v>5778215.248443971</v>
+        <v>5778215.24844397</v>
       </c>
       <c r="E282" t="n">
         <v>4404155319.48494</v>
       </c>
       <c r="F282" t="n">
-        <v>147617.992520163</v>
+        <v>147617.9925201628</v>
       </c>
       <c r="G282" t="n">
         <v>1913</v>
@@ -8913,13 +8913,13 @@
         </is>
       </c>
       <c r="D283" t="n">
-        <v>79025350.17698412</v>
+        <v>79025350.17698413</v>
       </c>
       <c r="E283" t="n">
-        <v>61627328366.01598</v>
+        <v>61627328366.01595</v>
       </c>
       <c r="F283" t="n">
-        <v>2059172.1594688</v>
+        <v>2059172.159468802</v>
       </c>
       <c r="G283" t="n">
         <v>2320</v>
@@ -8943,13 +8943,13 @@
         </is>
       </c>
       <c r="D284" t="n">
-        <v>9499772.824727917</v>
+        <v>9499772.824727915</v>
       </c>
       <c r="E284" t="n">
-        <v>7141830728.679981</v>
+        <v>7141830728.679982</v>
       </c>
       <c r="F284" t="n">
-        <v>240093.148264903</v>
+        <v>240093.1482649031</v>
       </c>
       <c r="G284" t="n">
         <v>4872</v>
@@ -8976,7 +8976,7 @@
         <v>53410517.96288092</v>
       </c>
       <c r="E285" t="n">
-        <v>40562332970.99297</v>
+        <v>40562332970.993</v>
       </c>
       <c r="F285" t="n">
         <v>1360027.979270707</v>
@@ -9003,13 +9003,13 @@
         </is>
       </c>
       <c r="D286" t="n">
-        <v>178419222.9196613</v>
+        <v>178419222.9196615</v>
       </c>
       <c r="E286" t="n">
-        <v>133735253504.5878</v>
+        <v>133735253504.5879</v>
       </c>
       <c r="F286" t="n">
-        <v>4502282.178884378</v>
+        <v>4502282.178884374</v>
       </c>
       <c r="G286" t="n">
         <v>38940</v>
@@ -9033,13 +9033,13 @@
         </is>
       </c>
       <c r="D287" t="n">
-        <v>181206471.6933506</v>
+        <v>181206471.6933508</v>
       </c>
       <c r="E287" t="n">
-        <v>135009220156.3274</v>
+        <v>135009220156.3273</v>
       </c>
       <c r="F287" t="n">
-        <v>4558184.544536342</v>
+        <v>4558184.544536348</v>
       </c>
       <c r="G287" t="n">
         <v>44242</v>
@@ -9063,13 +9063,13 @@
         </is>
       </c>
       <c r="D288" t="n">
-        <v>1698728.020470166</v>
+        <v>1698728.020470165</v>
       </c>
       <c r="E288" t="n">
         <v>1292629703.289689</v>
       </c>
       <c r="F288" t="n">
-        <v>43313.74381873183</v>
+        <v>43313.74381873184</v>
       </c>
       <c r="G288" t="n">
         <v>362</v>
@@ -9093,13 +9093,13 @@
         </is>
       </c>
       <c r="D289" t="n">
-        <v>3741641.138749395</v>
+        <v>3741641.138749393</v>
       </c>
       <c r="E289" t="n">
         <v>2786269458.506639</v>
       </c>
       <c r="F289" t="n">
-        <v>93912.29174144162</v>
+        <v>93912.29174144164</v>
       </c>
       <c r="G289" t="n">
         <v>1639</v>
@@ -9126,10 +9126,10 @@
         <v>121571633.0605613</v>
       </c>
       <c r="E290" t="n">
-        <v>90554572309.36525</v>
+        <v>90554572309.36517</v>
       </c>
       <c r="F290" t="n">
-        <v>3049679.426666238</v>
+        <v>3049679.426666241</v>
       </c>
       <c r="G290" t="n">
         <v>25476</v>
@@ -9156,10 +9156,10 @@
         <v>1863524.517793061</v>
       </c>
       <c r="E291" t="n">
-        <v>1385369926.950472</v>
+        <v>1385369926.950471</v>
       </c>
       <c r="F291" t="n">
-        <v>46807.57823139579</v>
+        <v>46807.57823139575</v>
       </c>
       <c r="G291" t="n">
         <v>255</v>
@@ -9219,7 +9219,7 @@
         <v>16543146484.5917</v>
       </c>
       <c r="F293" t="n">
-        <v>556589.3040314143</v>
+        <v>556589.3040314141</v>
       </c>
       <c r="G293" t="n">
         <v>5624</v>
@@ -9243,13 +9243,13 @@
         </is>
       </c>
       <c r="D294" t="n">
-        <v>63842491.20672244</v>
+        <v>63842491.20672262</v>
       </c>
       <c r="E294" t="n">
-        <v>47697694210.39537</v>
+        <v>47697694210.39538</v>
       </c>
       <c r="F294" t="n">
-        <v>1608507.522197555</v>
+        <v>1608507.522197563</v>
       </c>
       <c r="G294" t="n">
         <v>19172</v>
@@ -9276,10 +9276,10 @@
         <v>173234575.0994787</v>
       </c>
       <c r="E295" t="n">
-        <v>128524668285.8781</v>
+        <v>128524668285.878</v>
       </c>
       <c r="F295" t="n">
-        <v>4326617.607154425</v>
+        <v>4326617.607154427</v>
       </c>
       <c r="G295" t="n">
         <v>1597</v>
@@ -9333,13 +9333,13 @@
         </is>
       </c>
       <c r="D297" t="n">
-        <v>17806262.78424218</v>
+        <v>17806262.78424219</v>
       </c>
       <c r="E297" t="n">
         <v>13414670813.70333</v>
       </c>
       <c r="F297" t="n">
-        <v>450850.9938733922</v>
+        <v>450850.9938733926</v>
       </c>
       <c r="G297" t="n">
         <v>9412</v>
@@ -9396,7 +9396,7 @@
         <v>28307969.1754538</v>
       </c>
       <c r="E299" t="n">
-        <v>21345049741.50743</v>
+        <v>21345049741.5074</v>
       </c>
       <c r="F299" t="n">
         <v>719028.9662668395</v>
@@ -9423,13 +9423,13 @@
         </is>
       </c>
       <c r="D300" t="n">
-        <v>52659046.28076352</v>
+        <v>52659046.28076367</v>
       </c>
       <c r="E300" t="n">
-        <v>39272527528.40173</v>
+        <v>39272527528.40175</v>
       </c>
       <c r="F300" t="n">
-        <v>1324096.221400965</v>
+        <v>1324096.221400967</v>
       </c>
       <c r="G300" t="n">
         <v>17759</v>
@@ -9456,10 +9456,10 @@
         <v>1023825.881122758</v>
       </c>
       <c r="E301" t="n">
-        <v>752719515.616926</v>
+        <v>752719515.6169261</v>
       </c>
       <c r="F301" t="n">
-        <v>25651.83169301216</v>
+        <v>25651.83169301217</v>
       </c>
       <c r="G301" t="n">
         <v>115</v>
@@ -9483,13 +9483,13 @@
         </is>
       </c>
       <c r="D302" t="n">
-        <v>28441914.27243485</v>
+        <v>28441914.27243486</v>
       </c>
       <c r="E302" t="n">
-        <v>21443202519.25336</v>
+        <v>21443202519.25337</v>
       </c>
       <c r="F302" t="n">
-        <v>720404.8308444426</v>
+        <v>720404.8308444427</v>
       </c>
       <c r="G302" t="n">
         <v>6836</v>
@@ -9516,10 +9516,10 @@
         <v>282359.0383095733</v>
       </c>
       <c r="E303" t="n">
-        <v>215264719.988439</v>
+        <v>215264719.9884391</v>
       </c>
       <c r="F303" t="n">
-        <v>7210.469665451566</v>
+        <v>7210.469665451567</v>
       </c>
       <c r="G303" t="n">
         <v>336</v>
@@ -9543,13 +9543,13 @@
         </is>
       </c>
       <c r="D304" t="n">
-        <v>195654774.7724351</v>
+        <v>195654774.7724352</v>
       </c>
       <c r="E304" t="n">
         <v>146306926347.3134</v>
       </c>
       <c r="F304" t="n">
-        <v>4928442.326770681</v>
+        <v>4928442.326770682</v>
       </c>
       <c r="G304" t="n">
         <v>55174</v>
@@ -9576,10 +9576,10 @@
         <v>62828621.16926101</v>
       </c>
       <c r="E305" t="n">
-        <v>48247125936.09131</v>
+        <v>48247125936.09132</v>
       </c>
       <c r="F305" t="n">
-        <v>1616867.541116945</v>
+        <v>1616867.541116946</v>
       </c>
       <c r="G305" t="n">
         <v>1224</v>
@@ -9603,13 +9603,13 @@
         </is>
       </c>
       <c r="D306" t="n">
-        <v>333601.4387044832</v>
+        <v>333601.4387044833</v>
       </c>
       <c r="E306" t="n">
         <v>254006731.8988081</v>
       </c>
       <c r="F306" t="n">
-        <v>8497.868484118277</v>
+        <v>8497.868484118279</v>
       </c>
       <c r="G306" t="n">
         <v>77</v>
@@ -9633,7 +9633,7 @@
         </is>
       </c>
       <c r="D307" t="n">
-        <v>67754328.3932481</v>
+        <v>67754328.3932482</v>
       </c>
       <c r="E307" t="n">
         <v>50822571622.07664</v>
@@ -9663,13 +9663,13 @@
         </is>
       </c>
       <c r="D308" t="n">
-        <v>2907788.458807404</v>
+        <v>2907788.458807406</v>
       </c>
       <c r="E308" t="n">
-        <v>2199182471.99951</v>
+        <v>2199182471.999511</v>
       </c>
       <c r="F308" t="n">
-        <v>73788.72852191099</v>
+        <v>73788.72852191096</v>
       </c>
       <c r="G308" t="n">
         <v>1291</v>
@@ -9693,13 +9693,13 @@
         </is>
       </c>
       <c r="D309" t="n">
-        <v>161886888.2384939</v>
+        <v>161886888.238494</v>
       </c>
       <c r="E309" t="n">
-        <v>120729215488.1373</v>
+        <v>120729215488.1374</v>
       </c>
       <c r="F309" t="n">
-        <v>4073449.770196315</v>
+        <v>4073449.770196309</v>
       </c>
       <c r="G309" t="n">
         <v>48313</v>
@@ -9723,13 +9723,13 @@
         </is>
       </c>
       <c r="D310" t="n">
-        <v>3008419279.948641</v>
+        <v>3008419279.948644</v>
       </c>
       <c r="E310" t="n">
-        <v>2239107491237.038</v>
+        <v>2239107491237.036</v>
       </c>
       <c r="F310" t="n">
-        <v>75491638.39724046</v>
+        <v>75491638.39724043</v>
       </c>
       <c r="G310" t="n">
         <v>163573</v>
@@ -9753,13 +9753,13 @@
         </is>
       </c>
       <c r="D311" t="n">
-        <v>24024693.36727714</v>
+        <v>24024693.36727716</v>
       </c>
       <c r="E311" t="n">
-        <v>18636057696.31971</v>
+        <v>18636057696.31972</v>
       </c>
       <c r="F311" t="n">
-        <v>623426.8937763013</v>
+        <v>623426.8937763015</v>
       </c>
       <c r="G311" t="n">
         <v>2270</v>
@@ -9783,10 +9783,10 @@
         </is>
       </c>
       <c r="D312" t="n">
-        <v>720806880.0581805</v>
+        <v>720806880.0581801</v>
       </c>
       <c r="E312" t="n">
-        <v>542144917627.8721</v>
+        <v>542144917627.8723</v>
       </c>
       <c r="F312" t="n">
         <v>18258573.20429464</v>
@@ -9813,10 +9813,10 @@
         </is>
       </c>
       <c r="D313" t="n">
-        <v>2372485181.7777</v>
+        <v>2372485181.777701</v>
       </c>
       <c r="E313" t="n">
-        <v>1747735965983.505</v>
+        <v>1747735965983.504</v>
       </c>
       <c r="F313" t="n">
         <v>58982208.9856327</v>
@@ -9843,10 +9843,10 @@
         </is>
       </c>
       <c r="D314" t="n">
-        <v>436586228.9246325</v>
+        <v>436586228.9246336</v>
       </c>
       <c r="E314" t="n">
-        <v>325442037933.5087</v>
+        <v>325442037933.5083</v>
       </c>
       <c r="F314" t="n">
         <v>10991865.10760948</v>
@@ -9873,13 +9873,13 @@
         </is>
       </c>
       <c r="D315" t="n">
-        <v>806638951.3463446</v>
+        <v>806638951.3463444</v>
       </c>
       <c r="E315" t="n">
-        <v>605461041258.3229</v>
+        <v>605461041258.3223</v>
       </c>
       <c r="F315" t="n">
-        <v>20391910.37299057</v>
+        <v>20391910.37299054</v>
       </c>
       <c r="G315" t="n">
         <v>7156</v>
@@ -9906,10 +9906,10 @@
         <v>15679394.10036254</v>
       </c>
       <c r="E316" t="n">
-        <v>11872459478.18588</v>
+        <v>11872459478.18589</v>
       </c>
       <c r="F316" t="n">
-        <v>398504.2935520811</v>
+        <v>398504.2935520823</v>
       </c>
       <c r="G316" t="n">
         <v>2102</v>
@@ -9933,13 +9933,13 @@
         </is>
       </c>
       <c r="D317" t="n">
-        <v>73813074.47831403</v>
+        <v>73813074.47831394</v>
       </c>
       <c r="E317" t="n">
         <v>55126425068.04946</v>
       </c>
       <c r="F317" t="n">
-        <v>1857381.870756555</v>
+        <v>1857381.870756552</v>
       </c>
       <c r="G317" t="n">
         <v>24658</v>
@@ -9969,7 +9969,7 @@
         <v>940985599.0090103</v>
       </c>
       <c r="F318" t="n">
-        <v>31637.74870134741</v>
+        <v>31637.74870134742</v>
       </c>
       <c r="G318" t="n">
         <v>462</v>
@@ -9996,10 +9996,10 @@
         <v>68956604.69107625</v>
       </c>
       <c r="E319" t="n">
-        <v>53523530202.60059</v>
+        <v>53523530202.60057</v>
       </c>
       <c r="F319" t="n">
-        <v>1787174.729996077</v>
+        <v>1787174.729996075</v>
       </c>
       <c r="G319" t="n">
         <v>760</v>
@@ -10023,7 +10023,7 @@
         </is>
       </c>
       <c r="D320" t="n">
-        <v>76048.46284399845</v>
+        <v>76048.46284399844</v>
       </c>
       <c r="E320" t="n">
         <v>55307298.49095853</v>
@@ -10053,7 +10053,7 @@
         </is>
       </c>
       <c r="D321" t="n">
-        <v>19202750.99068797</v>
+        <v>19202750.99068796</v>
       </c>
       <c r="E321" t="n">
         <v>14468575532.67535</v>
@@ -10086,7 +10086,7 @@
         <v>95896631.04286174</v>
       </c>
       <c r="E322" t="n">
-        <v>71764647966.10133</v>
+        <v>71764647966.10132</v>
       </c>
       <c r="F322" t="n">
         <v>2416595.112419985</v>
@@ -10113,13 +10113,13 @@
         </is>
       </c>
       <c r="D323" t="n">
-        <v>380563.9950761086</v>
+        <v>380563.9950761088</v>
       </c>
       <c r="E323" t="n">
         <v>293174077.5792953</v>
       </c>
       <c r="F323" t="n">
-        <v>9772.675646938469</v>
+        <v>9772.675646938471</v>
       </c>
       <c r="G323" t="n">
         <v>262</v>
@@ -10146,10 +10146,10 @@
         <v>1233631.364320976</v>
       </c>
       <c r="E324" t="n">
-        <v>951417122.8997822</v>
+        <v>951417122.8997819</v>
       </c>
       <c r="F324" t="n">
-        <v>31775.42348130395</v>
+        <v>31775.42348130397</v>
       </c>
       <c r="G324" t="n">
         <v>255</v>
@@ -10176,7 +10176,7 @@
         <v>11649352.35157956</v>
       </c>
       <c r="E325" t="n">
-        <v>8902032131.195366</v>
+        <v>8902032131.19537</v>
       </c>
       <c r="F325" t="n">
         <v>298422.9376598292</v>
@@ -10233,10 +10233,10 @@
         </is>
       </c>
       <c r="D327" t="n">
-        <v>59147473.55198954</v>
+        <v>59147473.55198969</v>
       </c>
       <c r="E327" t="n">
-        <v>44496296795.58707</v>
+        <v>44496296795.58705</v>
       </c>
       <c r="F327" t="n">
         <v>1495988.514355836</v>
@@ -10263,10 +10263,10 @@
         </is>
       </c>
       <c r="D328" t="n">
-        <v>48088322.40857168</v>
+        <v>48088322.4085716</v>
       </c>
       <c r="E328" t="n">
-        <v>36076014683.1546</v>
+        <v>36076014683.15459</v>
       </c>
       <c r="F328" t="n">
         <v>1215334.953337948</v>
@@ -10293,10 +10293,10 @@
         </is>
       </c>
       <c r="D329" t="n">
-        <v>27495305.22085912</v>
+        <v>27495305.22085911</v>
       </c>
       <c r="E329" t="n">
-        <v>20610748912.8351</v>
+        <v>20610748912.83509</v>
       </c>
       <c r="F329" t="n">
         <v>692233.4968052419</v>
@@ -10323,13 +10323,13 @@
         </is>
       </c>
       <c r="D330" t="n">
-        <v>8434216.916792165</v>
+        <v>8434216.916792167</v>
       </c>
       <c r="E330" t="n">
-        <v>6332814936.630074</v>
+        <v>6332814936.630073</v>
       </c>
       <c r="F330" t="n">
-        <v>212922.2210151918</v>
+        <v>212922.2210151919</v>
       </c>
       <c r="G330" t="n">
         <v>4960</v>
@@ -10356,10 +10356,10 @@
         <v>120599081.6793514</v>
       </c>
       <c r="E331" t="n">
-        <v>90110982746.07001</v>
+        <v>90110982746.07007</v>
       </c>
       <c r="F331" t="n">
-        <v>3033970.455942745</v>
+        <v>3033970.455942746</v>
       </c>
       <c r="G331" t="n">
         <v>17025</v>
@@ -10383,7 +10383,7 @@
         </is>
       </c>
       <c r="D332" t="n">
-        <v>4877383.810542905</v>
+        <v>4877383.810542906</v>
       </c>
       <c r="E332" t="n">
         <v>3639580329.422746</v>
@@ -10413,13 +10413,13 @@
         </is>
       </c>
       <c r="D333" t="n">
-        <v>110202935.0817503</v>
+        <v>110202935.08175</v>
       </c>
       <c r="E333" t="n">
         <v>82815373763.05177</v>
       </c>
       <c r="F333" t="n">
-        <v>2786224.175024306</v>
+        <v>2786224.175024312</v>
       </c>
       <c r="G333" t="n">
         <v>28180</v>
@@ -10446,10 +10446,10 @@
         <v>11320793.91591047</v>
       </c>
       <c r="E334" t="n">
-        <v>8501000995.820887</v>
+        <v>8501000995.820889</v>
       </c>
       <c r="F334" t="n">
-        <v>285627.3348802344</v>
+        <v>285627.3348802347</v>
       </c>
       <c r="G334" t="n">
         <v>2057</v>
@@ -10476,10 +10476,10 @@
         <v>223901773.1575902</v>
       </c>
       <c r="E335" t="n">
-        <v>167788192454.7877</v>
+        <v>167788192454.7878</v>
       </c>
       <c r="F335" t="n">
-        <v>5653972.178649696</v>
+        <v>5653972.178649697</v>
       </c>
       <c r="G335" t="n">
         <v>49745</v>
@@ -10503,10 +10503,10 @@
         </is>
       </c>
       <c r="D336" t="n">
-        <v>247877287.5714845</v>
+        <v>247877287.5714847</v>
       </c>
       <c r="E336" t="n">
-        <v>185752837643.5479</v>
+        <v>185752837643.5478</v>
       </c>
       <c r="F336" t="n">
         <v>6253418.405499822</v>
@@ -10533,13 +10533,13 @@
         </is>
       </c>
       <c r="D337" t="n">
-        <v>99782868.14997078</v>
+        <v>99782868.14997087</v>
       </c>
       <c r="E337" t="n">
-        <v>74473296132.7682</v>
+        <v>74473296132.76822</v>
       </c>
       <c r="F337" t="n">
-        <v>2516382.429519362</v>
+        <v>2516382.429519364</v>
       </c>
       <c r="G337" t="n">
         <v>1764</v>

</xml_diff>